<commit_message>
correcting import with Configuration in ImportRequest
</commit_message>
<xml_diff>
--- a/modules/Insurance/Files/Microsoft/2026/Microsoft.xlsx
+++ b/modules/Insurance/Files/Microsoft/2026/Microsoft.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\MeshWeaver\modules\Insurance\Files\Microsoft\2026\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://systemorph-my.sharepoint.com/personal/rbuergi_systemorph_com/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37CFED4D-9876-4514-8893-9A71107E03D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{37CFED4D-9876-4514-8893-9A71107E03D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6A33AB4-E925-45BD-839C-BAEDD97ED29B}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16860" xr2:uid="{74B429DF-FE2F-4D9F-BEF1-C117811C90CF}"/>
+    <workbookView xWindow="6130" yWindow="3400" windowWidth="18720" windowHeight="12190" xr2:uid="{74B429DF-FE2F-4D9F-BEF1-C117811C90CF}"/>
   </bookViews>
   <sheets>
     <sheet name="2024 PDBI Values (Final)" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2024 PDBI Values (Final)'!$B$1:$R$74</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2024 PDBI Values (Final)'!$B$1:$R$73</definedName>
     <definedName name="QuickView_QuickView1">#REF!</definedName>
     <definedName name="QuickView_QuickView1_ColHeader">#REF!</definedName>
     <definedName name="QuickView_QuickView1_Data">#REF!</definedName>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="254">
   <si>
     <t>Currency: GBP</t>
   </si>
@@ -182,15 +182,6 @@
   </si>
   <si>
     <t>Taiwan</t>
-  </si>
-  <si>
-    <t>TWOF</t>
-  </si>
-  <si>
-    <t>Taipei, Taiwan</t>
-  </si>
-  <si>
-    <t>Unit 407, Level 4, Neihu New Century Building, No. 55, Zhouzi Street, Neihu District, Taipei 114, Taiwan</t>
   </si>
   <si>
     <t>Total (GBP)</t>
@@ -841,7 +832,7 @@
     <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="&quot;£&quot;#,##0"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -860,14 +851,6 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -984,10 +967,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1004,36 +987,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1041,16 +1011,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1070,10 +1040,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1376,11 +1342,11 @@
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:AU81"/>
+  <dimension ref="A1:AU80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelRow="1"/>
@@ -1403,36 +1369,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18.5">
-      <c r="B1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="12"/>
+      <c r="B1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10"/>
       <c r="Q1" s="4"/>
     </row>
     <row r="2" spans="1:18" ht="18.5">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="10">
-        <f>Q73</f>
+      <c r="C2" s="8">
+        <f>Q72</f>
         <v>802580000</v>
       </c>
       <c r="Q2" s="4"/>
     </row>
     <row r="3" spans="1:18" ht="18.5">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="8">
         <v>5237100057</v>
       </c>
       <c r="Q3" s="4"/>
     </row>
     <row r="4" spans="1:18" ht="18.5">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="16">
         <f>SUM(C2:C3)</f>
         <v>6039680057</v>
       </c>
@@ -1440,298 +1406,301 @@
     </row>
     <row r="5" spans="1:18" customFormat="1"/>
     <row r="6" spans="1:18" s="6" customFormat="1" ht="18.5">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="J6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="K6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="L6" s="14" t="s">
+      <c r="L6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="M6" s="14" t="s">
+      <c r="M6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="N6" s="14" t="s">
+      <c r="N6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="O6" s="14" t="s">
+      <c r="O6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="P6" s="14" t="s">
+      <c r="P6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="Q6" s="14" t="s">
+      <c r="Q6" s="11" t="s">
         <v>19</v>
       </c>
       <c r="R6"/>
     </row>
-    <row r="7" spans="1:18" ht="14.5" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="B7" s="8"/>
-      <c r="C7" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="15" t="s">
+    <row r="7" spans="1:18" customFormat="1">
+      <c r="A7" s="4"/>
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="16" t="s">
+      <c r="E7" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="13">
-        <v>0</v>
-      </c>
-      <c r="H7" s="13">
-        <v>0</v>
-      </c>
-      <c r="I7" s="13">
-        <v>0</v>
-      </c>
-      <c r="J7" s="13">
-        <v>0</v>
-      </c>
-      <c r="K7" s="13">
-        <v>0</v>
-      </c>
-      <c r="L7" s="13">
-        <v>0</v>
-      </c>
-      <c r="M7" s="13">
-        <v>0</v>
-      </c>
-      <c r="N7" s="13">
-        <v>0</v>
-      </c>
-      <c r="O7" s="13">
-        <v>0</v>
-      </c>
-      <c r="P7" s="13">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="13">
-        <f t="shared" ref="Q7" si="0">G7+H7+I7+J7+K7+L7+M7+N7+O7+P7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" customFormat="1" collapsed="1">
+      <c r="F7" t="s">
+        <v>127</v>
+      </c>
+      <c r="G7">
+        <v>125000000</v>
+      </c>
+      <c r="H7">
+        <v>45000000</v>
+      </c>
+      <c r="I7">
+        <v>12000000</v>
+      </c>
+      <c r="J7">
+        <v>8500000</v>
+      </c>
+      <c r="K7">
+        <v>15000000</v>
+      </c>
+      <c r="L7">
+        <v>18000000</v>
+      </c>
+      <c r="M7">
+        <v>22000000</v>
+      </c>
+      <c r="N7">
+        <v>3500000</v>
+      </c>
+      <c r="O7">
+        <v>1000000</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <f>SUM(G7:P7)</f>
+        <v>250000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" customFormat="1">
       <c r="A8" s="4"/>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D8" t="s">
         <v>45</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="F8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G8">
-        <v>125000000</v>
+        <v>8500000</v>
       </c>
       <c r="H8">
-        <v>45000000</v>
+        <v>3200000</v>
       </c>
       <c r="I8">
-        <v>12000000</v>
+        <v>850000</v>
       </c>
       <c r="J8">
-        <v>8500000</v>
+        <v>650000</v>
       </c>
       <c r="K8">
-        <v>15000000</v>
+        <v>2500000</v>
       </c>
       <c r="L8">
-        <v>18000000</v>
+        <v>1200000</v>
       </c>
       <c r="M8">
-        <v>22000000</v>
+        <v>1800000</v>
       </c>
       <c r="N8">
-        <v>3500000</v>
+        <v>0</v>
       </c>
       <c r="O8">
-        <v>1000000</v>
+        <v>300000</v>
       </c>
       <c r="P8">
-        <v>0</v>
+        <v>2400000</v>
       </c>
       <c r="Q8">
-        <f>SUM(G8:P8)</f>
-        <v>250000000</v>
+        <f t="shared" ref="Q8:Q70" si="0">SUM(G8:P8)</f>
+        <v>21400000</v>
       </c>
     </row>
     <row r="9" spans="1:18" customFormat="1">
       <c r="A9" s="4"/>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
         <v>21</v>
       </c>
       <c r="F9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G9">
-        <v>8500000</v>
+        <v>12000000</v>
       </c>
       <c r="H9">
-        <v>3200000</v>
+        <v>4500000</v>
       </c>
       <c r="I9">
-        <v>850000</v>
+        <v>1100000</v>
       </c>
       <c r="J9">
-        <v>650000</v>
+        <v>950000</v>
       </c>
       <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>2200000</v>
+      </c>
+      <c r="M9">
         <v>2500000</v>
       </c>
-      <c r="L9">
-        <v>1200000</v>
-      </c>
-      <c r="M9">
-        <v>1800000</v>
-      </c>
       <c r="N9">
         <v>0</v>
       </c>
       <c r="O9">
-        <v>300000</v>
+        <v>750000</v>
       </c>
       <c r="P9">
-        <v>2400000</v>
+        <v>4800000</v>
       </c>
       <c r="Q9">
-        <f t="shared" ref="Q9:Q71" si="1">SUM(G9:P9)</f>
-        <v>21400000</v>
+        <f t="shared" si="0"/>
+        <v>28800000</v>
       </c>
     </row>
     <row r="10" spans="1:18" customFormat="1">
       <c r="A10" s="4"/>
       <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" t="s">
+        <v>132</v>
+      </c>
+      <c r="D10" t="s">
         <v>47</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" t="s">
         <v>133</v>
       </c>
-      <c r="D10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" t="s">
-        <v>134</v>
-      </c>
       <c r="G10">
-        <v>12000000</v>
+        <v>2100000</v>
       </c>
       <c r="H10">
-        <v>4500000</v>
+        <v>800000</v>
       </c>
       <c r="I10">
-        <v>1100000</v>
+        <v>220000</v>
       </c>
       <c r="J10">
-        <v>950000</v>
+        <v>450000</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <v>1200000</v>
       </c>
       <c r="L10">
-        <v>2200000</v>
+        <v>430000</v>
       </c>
       <c r="M10">
-        <v>2500000</v>
+        <v>0</v>
       </c>
       <c r="N10">
         <v>0</v>
       </c>
       <c r="O10">
-        <v>750000</v>
+        <v>0</v>
       </c>
       <c r="P10">
-        <v>4800000</v>
+        <v>1200000</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="1"/>
-        <v>28800000</v>
+        <f t="shared" si="0"/>
+        <v>6400000</v>
       </c>
     </row>
     <row r="11" spans="1:18" customFormat="1">
       <c r="A11" s="4"/>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
+        <v>134</v>
+      </c>
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" t="s">
         <v>135</v>
       </c>
-      <c r="D11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" t="s">
-        <v>136</v>
-      </c>
       <c r="G11">
-        <v>2100000</v>
+        <v>2800000</v>
       </c>
       <c r="H11">
-        <v>800000</v>
+        <v>1050000</v>
       </c>
       <c r="I11">
-        <v>220000</v>
+        <v>280000</v>
       </c>
       <c r="J11">
-        <v>450000</v>
+        <v>320000</v>
       </c>
       <c r="K11">
-        <v>1200000</v>
+        <v>0</v>
       </c>
       <c r="L11">
-        <v>430000</v>
+        <v>650000</v>
       </c>
       <c r="M11">
-        <v>0</v>
+        <v>500000</v>
       </c>
       <c r="N11">
         <v>0</v>
@@ -1740,11 +1709,11 @@
         <v>0</v>
       </c>
       <c r="P11">
-        <v>1200000</v>
+        <v>1800000</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="1"/>
-        <v>6400000</v>
+        <f t="shared" si="0"/>
+        <v>7400000</v>
       </c>
     </row>
     <row r="12" spans="1:18" customFormat="1">
@@ -1753,37 +1722,37 @@
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E12" t="s">
         <v>21</v>
       </c>
       <c r="F12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G12">
-        <v>2800000</v>
+        <v>4200000</v>
       </c>
       <c r="H12">
-        <v>1050000</v>
+        <v>1600000</v>
       </c>
       <c r="I12">
-        <v>280000</v>
+        <v>420000</v>
       </c>
       <c r="J12">
-        <v>320000</v>
+        <v>480000</v>
       </c>
       <c r="K12">
-        <v>0</v>
+        <v>900000</v>
       </c>
       <c r="L12">
-        <v>650000</v>
+        <v>800000</v>
       </c>
       <c r="M12">
-        <v>500000</v>
+        <v>1000000</v>
       </c>
       <c r="N12">
         <v>0</v>
@@ -1792,50 +1761,50 @@
         <v>0</v>
       </c>
       <c r="P12">
-        <v>1800000</v>
+        <v>2200000</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="1"/>
-        <v>7400000</v>
+        <f t="shared" si="0"/>
+        <v>11600000</v>
       </c>
     </row>
     <row r="13" spans="1:18" customFormat="1">
       <c r="A13" s="4"/>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
+        <v>138</v>
+      </c>
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" t="s">
         <v>139</v>
       </c>
-      <c r="D13" t="s">
-        <v>53</v>
-      </c>
-      <c r="E13" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" t="s">
-        <v>140</v>
-      </c>
       <c r="G13">
-        <v>4200000</v>
+        <v>950000</v>
       </c>
       <c r="H13">
-        <v>1600000</v>
+        <v>280000</v>
       </c>
       <c r="I13">
+        <v>50000</v>
+      </c>
+      <c r="J13">
         <v>420000</v>
       </c>
-      <c r="J13">
-        <v>480000</v>
-      </c>
       <c r="K13">
-        <v>900000</v>
+        <v>200000</v>
       </c>
       <c r="L13">
-        <v>800000</v>
+        <v>0</v>
       </c>
       <c r="M13">
-        <v>1000000</v>
+        <v>0</v>
       </c>
       <c r="N13">
         <v>0</v>
@@ -1844,47 +1813,47 @@
         <v>0</v>
       </c>
       <c r="P13">
-        <v>2200000</v>
+        <v>0</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="1"/>
-        <v>11600000</v>
+        <f t="shared" si="0"/>
+        <v>1900000</v>
       </c>
     </row>
     <row r="14" spans="1:18" customFormat="1">
       <c r="A14" s="4"/>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
+        <v>140</v>
+      </c>
+      <c r="D14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" t="s">
         <v>141</v>
       </c>
-      <c r="D14" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" t="s">
-        <v>55</v>
-      </c>
-      <c r="F14" t="s">
-        <v>142</v>
-      </c>
       <c r="G14">
-        <v>950000</v>
+        <v>2400000</v>
       </c>
       <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>180000</v>
+      </c>
+      <c r="J14">
         <v>280000</v>
       </c>
-      <c r="I14">
-        <v>50000</v>
-      </c>
-      <c r="J14">
-        <v>420000</v>
-      </c>
       <c r="K14">
-        <v>200000</v>
+        <v>0</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>220000</v>
       </c>
       <c r="M14">
         <v>0</v>
@@ -1896,47 +1865,47 @@
         <v>0</v>
       </c>
       <c r="P14">
-        <v>0</v>
+        <v>1500000</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="1"/>
-        <v>1900000</v>
+        <f t="shared" si="0"/>
+        <v>4580000</v>
       </c>
     </row>
     <row r="15" spans="1:18" customFormat="1">
       <c r="A15" s="4"/>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
+        <v>142</v>
+      </c>
+      <c r="D15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" t="s">
         <v>143</v>
       </c>
-      <c r="D15" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" t="s">
-        <v>57</v>
-      </c>
-      <c r="F15" t="s">
-        <v>144</v>
-      </c>
       <c r="G15">
-        <v>2400000</v>
+        <v>1100000</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>320000</v>
       </c>
       <c r="I15">
-        <v>180000</v>
+        <v>45000</v>
       </c>
       <c r="J15">
-        <v>280000</v>
+        <v>480000</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>255000</v>
       </c>
       <c r="L15">
-        <v>220000</v>
+        <v>0</v>
       </c>
       <c r="M15">
         <v>0</v>
@@ -1948,47 +1917,47 @@
         <v>0</v>
       </c>
       <c r="P15">
-        <v>1500000</v>
+        <v>0</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="1"/>
-        <v>4580000</v>
+        <f t="shared" si="0"/>
+        <v>2200000</v>
       </c>
     </row>
     <row r="16" spans="1:18" customFormat="1">
       <c r="A16" s="4"/>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
+        <v>144</v>
+      </c>
+      <c r="D16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" t="s">
         <v>145</v>
       </c>
-      <c r="D16" t="s">
-        <v>58</v>
-      </c>
-      <c r="E16" t="s">
-        <v>55</v>
-      </c>
-      <c r="F16" t="s">
-        <v>146</v>
-      </c>
       <c r="G16">
-        <v>1100000</v>
+        <v>1600000</v>
       </c>
       <c r="H16">
-        <v>320000</v>
+        <v>0</v>
       </c>
       <c r="I16">
-        <v>45000</v>
+        <v>150000</v>
       </c>
       <c r="J16">
-        <v>480000</v>
+        <v>220000</v>
       </c>
       <c r="K16">
-        <v>255000</v>
+        <v>0</v>
       </c>
       <c r="L16">
-        <v>0</v>
+        <v>180000</v>
       </c>
       <c r="M16">
         <v>0</v>
@@ -2000,154 +1969,154 @@
         <v>0</v>
       </c>
       <c r="P16">
-        <v>0</v>
+        <v>950000</v>
       </c>
       <c r="Q16">
-        <f t="shared" si="1"/>
-        <v>2200000</v>
+        <f t="shared" si="0"/>
+        <v>3100000</v>
       </c>
     </row>
     <row r="17" spans="1:17" customFormat="1">
       <c r="A17" s="4"/>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
+        <v>146</v>
+      </c>
+      <c r="D17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" t="s">
         <v>147</v>
       </c>
-      <c r="D17" t="s">
-        <v>59</v>
-      </c>
-      <c r="E17" t="s">
-        <v>57</v>
-      </c>
-      <c r="F17" t="s">
-        <v>148</v>
-      </c>
       <c r="G17">
-        <v>1600000</v>
+        <v>15000000</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>5500000</v>
       </c>
       <c r="I17">
-        <v>150000</v>
+        <v>1400000</v>
       </c>
       <c r="J17">
-        <v>220000</v>
+        <v>1200000</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
       <c r="L17">
-        <v>180000</v>
+        <v>2800000</v>
       </c>
       <c r="M17">
-        <v>0</v>
+        <v>3200000</v>
       </c>
       <c r="N17">
         <v>0</v>
       </c>
       <c r="O17">
-        <v>0</v>
+        <v>900000</v>
       </c>
       <c r="P17">
-        <v>950000</v>
+        <v>6500000</v>
       </c>
       <c r="Q17">
-        <f t="shared" si="1"/>
-        <v>3100000</v>
+        <f t="shared" si="0"/>
+        <v>36500000</v>
       </c>
     </row>
     <row r="18" spans="1:17" customFormat="1">
       <c r="A18" s="4"/>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E18" t="s">
         <v>21</v>
       </c>
       <c r="F18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G18">
-        <v>15000000</v>
+        <v>7800000</v>
       </c>
       <c r="H18">
-        <v>5500000</v>
+        <v>2900000</v>
       </c>
       <c r="I18">
+        <v>780000</v>
+      </c>
+      <c r="J18">
+        <v>920000</v>
+      </c>
+      <c r="K18">
+        <v>1800000</v>
+      </c>
+      <c r="L18">
         <v>1400000</v>
       </c>
-      <c r="J18">
-        <v>1200000</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>2800000</v>
-      </c>
       <c r="M18">
-        <v>3200000</v>
+        <v>0</v>
       </c>
       <c r="N18">
         <v>0</v>
       </c>
       <c r="O18">
-        <v>900000</v>
+        <v>0</v>
       </c>
       <c r="P18">
-        <v>6500000</v>
+        <v>2100000</v>
       </c>
       <c r="Q18">
-        <f t="shared" si="1"/>
-        <v>36500000</v>
+        <f t="shared" si="0"/>
+        <v>17700000</v>
       </c>
     </row>
     <row r="19" spans="1:17" customFormat="1">
       <c r="A19" s="4"/>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E19" t="s">
         <v>21</v>
       </c>
       <c r="F19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G19">
-        <v>7800000</v>
+        <v>6500000</v>
       </c>
       <c r="H19">
-        <v>2900000</v>
+        <v>2400000</v>
       </c>
       <c r="I19">
-        <v>780000</v>
+        <v>650000</v>
       </c>
       <c r="J19">
-        <v>920000</v>
+        <v>750000</v>
       </c>
       <c r="K19">
-        <v>1800000</v>
+        <v>0</v>
       </c>
       <c r="L19">
-        <v>1400000</v>
+        <v>1200000</v>
       </c>
       <c r="M19">
-        <v>0</v>
+        <v>1500000</v>
       </c>
       <c r="N19">
         <v>0</v>
@@ -2156,50 +2125,50 @@
         <v>0</v>
       </c>
       <c r="P19">
-        <v>2100000</v>
+        <v>3200000</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="1"/>
-        <v>17700000</v>
+        <f t="shared" si="0"/>
+        <v>16200000</v>
       </c>
     </row>
     <row r="20" spans="1:17" customFormat="1">
       <c r="A20" s="4"/>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E20" t="s">
         <v>21</v>
       </c>
       <c r="F20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G20">
-        <v>6500000</v>
+        <v>9200000</v>
       </c>
       <c r="H20">
-        <v>2400000</v>
+        <v>3400000</v>
       </c>
       <c r="I20">
-        <v>650000</v>
+        <v>920000</v>
       </c>
       <c r="J20">
-        <v>750000</v>
+        <v>1050000</v>
       </c>
       <c r="K20">
-        <v>0</v>
+        <v>2100000</v>
       </c>
       <c r="L20">
-        <v>1200000</v>
+        <v>1730000</v>
       </c>
       <c r="M20">
-        <v>1500000</v>
+        <v>0</v>
       </c>
       <c r="N20">
         <v>0</v>
@@ -2208,50 +2177,50 @@
         <v>0</v>
       </c>
       <c r="P20">
-        <v>3200000</v>
+        <v>2800000</v>
       </c>
       <c r="Q20">
-        <f t="shared" si="1"/>
-        <v>16200000</v>
+        <f t="shared" si="0"/>
+        <v>21200000</v>
       </c>
     </row>
     <row r="21" spans="1:17" customFormat="1">
       <c r="A21" s="4"/>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E21" t="s">
         <v>21</v>
       </c>
       <c r="F21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G21">
-        <v>9200000</v>
+        <v>3400000</v>
       </c>
       <c r="H21">
-        <v>3400000</v>
+        <v>1250000</v>
       </c>
       <c r="I21">
-        <v>920000</v>
+        <v>340000</v>
       </c>
       <c r="J21">
-        <v>1050000</v>
+        <v>420000</v>
       </c>
       <c r="K21">
-        <v>2100000</v>
+        <v>0</v>
       </c>
       <c r="L21">
-        <v>1730000</v>
+        <v>890000</v>
       </c>
       <c r="M21">
-        <v>0</v>
+        <v>500000</v>
       </c>
       <c r="N21">
         <v>0</v>
@@ -2260,50 +2229,50 @@
         <v>0</v>
       </c>
       <c r="P21">
-        <v>2800000</v>
+        <v>1900000</v>
       </c>
       <c r="Q21">
-        <f t="shared" si="1"/>
-        <v>21200000</v>
+        <f t="shared" si="0"/>
+        <v>8700000</v>
       </c>
     </row>
     <row r="22" spans="1:17" customFormat="1">
       <c r="A22" s="4"/>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E22" t="s">
         <v>21</v>
       </c>
       <c r="F22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G22">
-        <v>3400000</v>
+        <v>2900000</v>
       </c>
       <c r="H22">
-        <v>1250000</v>
+        <v>1100000</v>
       </c>
       <c r="I22">
-        <v>340000</v>
+        <v>290000</v>
       </c>
       <c r="J22">
-        <v>420000</v>
+        <v>350000</v>
       </c>
       <c r="K22">
-        <v>0</v>
+        <v>680000</v>
       </c>
       <c r="L22">
-        <v>890000</v>
+        <v>480000</v>
       </c>
       <c r="M22">
-        <v>500000</v>
+        <v>0</v>
       </c>
       <c r="N22">
         <v>0</v>
@@ -2312,50 +2281,50 @@
         <v>0</v>
       </c>
       <c r="P22">
-        <v>1900000</v>
+        <v>1600000</v>
       </c>
       <c r="Q22">
-        <f t="shared" si="1"/>
-        <v>8700000</v>
+        <f t="shared" si="0"/>
+        <v>7400000</v>
       </c>
     </row>
     <row r="23" spans="1:17" customFormat="1">
       <c r="A23" s="4"/>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E23" t="s">
         <v>21</v>
       </c>
       <c r="F23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G23">
-        <v>2900000</v>
+        <v>2200000</v>
       </c>
       <c r="H23">
-        <v>1100000</v>
+        <v>820000</v>
       </c>
       <c r="I23">
-        <v>290000</v>
+        <v>220000</v>
       </c>
       <c r="J23">
-        <v>350000</v>
+        <v>280000</v>
       </c>
       <c r="K23">
-        <v>680000</v>
+        <v>0</v>
       </c>
       <c r="L23">
-        <v>480000</v>
+        <v>580000</v>
       </c>
       <c r="M23">
-        <v>0</v>
+        <v>300000</v>
       </c>
       <c r="N23">
         <v>0</v>
@@ -2364,50 +2333,50 @@
         <v>0</v>
       </c>
       <c r="P23">
-        <v>1600000</v>
+        <v>1400000</v>
       </c>
       <c r="Q23">
-        <f t="shared" si="1"/>
-        <v>7400000</v>
+        <f t="shared" si="0"/>
+        <v>5800000</v>
       </c>
     </row>
     <row r="24" spans="1:17" customFormat="1">
       <c r="A24" s="4"/>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s">
+        <v>160</v>
+      </c>
+      <c r="D24" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" t="s">
+        <v>52</v>
+      </c>
+      <c r="F24" t="s">
         <v>161</v>
       </c>
-      <c r="D24" t="s">
-        <v>66</v>
-      </c>
-      <c r="E24" t="s">
-        <v>21</v>
-      </c>
-      <c r="F24" t="s">
-        <v>162</v>
-      </c>
       <c r="G24">
-        <v>2200000</v>
+        <v>680000</v>
       </c>
       <c r="H24">
-        <v>820000</v>
+        <v>200000</v>
       </c>
       <c r="I24">
-        <v>220000</v>
+        <v>35000</v>
       </c>
       <c r="J24">
-        <v>280000</v>
+        <v>310000</v>
       </c>
       <c r="K24">
-        <v>0</v>
+        <v>135000</v>
       </c>
       <c r="L24">
-        <v>580000</v>
+        <v>0</v>
       </c>
       <c r="M24">
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="N24">
         <v>0</v>
@@ -2416,44 +2385,44 @@
         <v>0</v>
       </c>
       <c r="P24">
-        <v>1400000</v>
+        <v>0</v>
       </c>
       <c r="Q24">
-        <f t="shared" si="1"/>
-        <v>5800000</v>
+        <f t="shared" si="0"/>
+        <v>1360000</v>
       </c>
     </row>
     <row r="25" spans="1:17" customFormat="1">
       <c r="A25" s="4"/>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C25" t="s">
+        <v>162</v>
+      </c>
+      <c r="D25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E25" t="s">
+        <v>52</v>
+      </c>
+      <c r="F25" t="s">
         <v>163</v>
       </c>
-      <c r="D25" t="s">
-        <v>67</v>
-      </c>
-      <c r="E25" t="s">
-        <v>55</v>
-      </c>
-      <c r="F25" t="s">
-        <v>164</v>
-      </c>
       <c r="G25">
-        <v>680000</v>
+        <v>820000</v>
       </c>
       <c r="H25">
-        <v>200000</v>
+        <v>240000</v>
       </c>
       <c r="I25">
-        <v>35000</v>
+        <v>40000</v>
       </c>
       <c r="J25">
-        <v>310000</v>
+        <v>370000</v>
       </c>
       <c r="K25">
-        <v>135000</v>
+        <v>170000</v>
       </c>
       <c r="L25">
         <v>0</v>
@@ -2471,47 +2440,47 @@
         <v>0</v>
       </c>
       <c r="Q25">
-        <f t="shared" si="1"/>
-        <v>1360000</v>
+        <f t="shared" si="0"/>
+        <v>1640000</v>
       </c>
     </row>
     <row r="26" spans="1:17" customFormat="1">
       <c r="A26" s="4"/>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C26" t="s">
+        <v>164</v>
+      </c>
+      <c r="D26" t="s">
+        <v>66</v>
+      </c>
+      <c r="E26" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" t="s">
         <v>165</v>
       </c>
-      <c r="D26" t="s">
-        <v>68</v>
-      </c>
-      <c r="E26" t="s">
-        <v>55</v>
-      </c>
-      <c r="F26" t="s">
-        <v>166</v>
-      </c>
       <c r="G26">
-        <v>820000</v>
+        <v>3100000</v>
       </c>
       <c r="H26">
-        <v>240000</v>
+        <v>1150000</v>
       </c>
       <c r="I26">
-        <v>40000</v>
+        <v>310000</v>
       </c>
       <c r="J26">
-        <v>370000</v>
+        <v>380000</v>
       </c>
       <c r="K26">
-        <v>170000</v>
+        <v>0</v>
       </c>
       <c r="L26">
-        <v>0</v>
+        <v>760000</v>
       </c>
       <c r="M26">
-        <v>0</v>
+        <v>500000</v>
       </c>
       <c r="N26">
         <v>0</v>
@@ -2520,50 +2489,50 @@
         <v>0</v>
       </c>
       <c r="P26">
-        <v>0</v>
+        <v>1800000</v>
       </c>
       <c r="Q26">
-        <f t="shared" si="1"/>
-        <v>1640000</v>
+        <f t="shared" si="0"/>
+        <v>8000000</v>
       </c>
     </row>
     <row r="27" spans="1:17" customFormat="1">
       <c r="A27" s="4"/>
       <c r="B27" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D27" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E27" t="s">
         <v>21</v>
       </c>
       <c r="F27" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G27">
-        <v>3100000</v>
+        <v>18000000</v>
       </c>
       <c r="H27">
-        <v>1150000</v>
+        <v>6500000</v>
       </c>
       <c r="I27">
-        <v>310000</v>
+        <v>1800000</v>
       </c>
       <c r="J27">
-        <v>380000</v>
+        <v>2100000</v>
       </c>
       <c r="K27">
-        <v>0</v>
+        <v>4200000</v>
       </c>
       <c r="L27">
-        <v>760000</v>
+        <v>3400000</v>
       </c>
       <c r="M27">
-        <v>500000</v>
+        <v>0</v>
       </c>
       <c r="N27">
         <v>0</v>
@@ -2572,11 +2541,11 @@
         <v>0</v>
       </c>
       <c r="P27">
-        <v>1800000</v>
+        <v>4500000</v>
       </c>
       <c r="Q27">
-        <f t="shared" si="1"/>
-        <v>8000000</v>
+        <f t="shared" si="0"/>
+        <v>40500000</v>
       </c>
     </row>
     <row r="28" spans="1:17" customFormat="1">
@@ -2585,34 +2554,34 @@
         <v>34</v>
       </c>
       <c r="C28" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D28" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E28" t="s">
         <v>21</v>
       </c>
       <c r="F28" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G28">
-        <v>18000000</v>
+        <v>12500000</v>
       </c>
       <c r="H28">
-        <v>6500000</v>
+        <v>4600000</v>
       </c>
       <c r="I28">
-        <v>1800000</v>
+        <v>1250000</v>
       </c>
       <c r="J28">
-        <v>2100000</v>
+        <v>1480000</v>
       </c>
       <c r="K28">
-        <v>4200000</v>
+        <v>2800000</v>
       </c>
       <c r="L28">
-        <v>3400000</v>
+        <v>2370000</v>
       </c>
       <c r="M28">
         <v>0</v>
@@ -2624,11 +2593,11 @@
         <v>0</v>
       </c>
       <c r="P28">
-        <v>4500000</v>
+        <v>3200000</v>
       </c>
       <c r="Q28">
-        <f t="shared" si="1"/>
-        <v>40500000</v>
+        <f t="shared" si="0"/>
+        <v>28200000</v>
       </c>
     </row>
     <row r="29" spans="1:17" customFormat="1">
@@ -2637,34 +2606,34 @@
         <v>34</v>
       </c>
       <c r="C29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E29" t="s">
         <v>21</v>
       </c>
       <c r="F29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G29">
-        <v>12500000</v>
+        <v>7200000</v>
       </c>
       <c r="H29">
-        <v>4600000</v>
+        <v>2650000</v>
       </c>
       <c r="I29">
-        <v>1250000</v>
+        <v>720000</v>
       </c>
       <c r="J29">
-        <v>1480000</v>
+        <v>850000</v>
       </c>
       <c r="K29">
-        <v>2800000</v>
+        <v>1800000</v>
       </c>
       <c r="L29">
-        <v>2370000</v>
+        <v>1180000</v>
       </c>
       <c r="M29">
         <v>0</v>
@@ -2676,51 +2645,51 @@
         <v>0</v>
       </c>
       <c r="P29">
-        <v>3200000</v>
+        <v>2100000</v>
       </c>
       <c r="Q29">
-        <f t="shared" si="1"/>
-        <v>28200000</v>
+        <f t="shared" si="0"/>
+        <v>16500000</v>
       </c>
     </row>
     <row r="30" spans="1:17" customFormat="1">
       <c r="A30" s="4"/>
       <c r="B30" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C30" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D30" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E30" t="s">
         <v>21</v>
       </c>
       <c r="F30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G30">
-        <v>7200000</v>
+        <v>9800000</v>
       </c>
       <c r="H30">
-        <v>2650000</v>
+        <v>3600000</v>
       </c>
       <c r="I30">
-        <v>720000</v>
+        <v>980000</v>
       </c>
       <c r="J30">
-        <v>850000</v>
+        <v>1150000</v>
       </c>
       <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <v>2270000</v>
+      </c>
+      <c r="M30">
         <v>1800000</v>
       </c>
-      <c r="L30">
-        <v>1180000</v>
-      </c>
-      <c r="M30">
-        <v>0</v>
-      </c>
       <c r="N30">
         <v>0</v>
       </c>
@@ -2728,11 +2697,11 @@
         <v>0</v>
       </c>
       <c r="P30">
-        <v>2100000</v>
+        <v>5200000</v>
       </c>
       <c r="Q30">
-        <f t="shared" si="1"/>
-        <v>16500000</v>
+        <f t="shared" si="0"/>
+        <v>24800000</v>
       </c>
     </row>
     <row r="31" spans="1:17" customFormat="1">
@@ -2741,89 +2710,89 @@
         <v>35</v>
       </c>
       <c r="C31" t="s">
+        <v>174</v>
+      </c>
+      <c r="D31" t="s">
+        <v>71</v>
+      </c>
+      <c r="E31" t="s">
+        <v>54</v>
+      </c>
+      <c r="F31" t="s">
         <v>175</v>
       </c>
-      <c r="D31" t="s">
-        <v>73</v>
-      </c>
-      <c r="E31" t="s">
-        <v>21</v>
-      </c>
-      <c r="F31" t="s">
-        <v>176</v>
-      </c>
       <c r="G31">
-        <v>9800000</v>
+        <v>2600000</v>
       </c>
       <c r="H31">
-        <v>3600000</v>
+        <v>0</v>
       </c>
       <c r="I31">
-        <v>980000</v>
+        <v>280000</v>
       </c>
       <c r="J31">
-        <v>1150000</v>
+        <v>380000</v>
       </c>
       <c r="K31">
         <v>0</v>
       </c>
       <c r="L31">
-        <v>2270000</v>
+        <v>440000</v>
       </c>
       <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31">
         <v>1800000</v>
       </c>
-      <c r="N31">
-        <v>0</v>
-      </c>
-      <c r="O31">
-        <v>0</v>
-      </c>
-      <c r="P31">
-        <v>5200000</v>
-      </c>
       <c r="Q31">
-        <f t="shared" si="1"/>
-        <v>24800000</v>
+        <f t="shared" si="0"/>
+        <v>5500000</v>
       </c>
     </row>
     <row r="32" spans="1:17" customFormat="1">
       <c r="A32" s="4"/>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C32" t="s">
+        <v>176</v>
+      </c>
+      <c r="D32" t="s">
+        <v>72</v>
+      </c>
+      <c r="E32" t="s">
+        <v>21</v>
+      </c>
+      <c r="F32" t="s">
         <v>177</v>
       </c>
-      <c r="D32" t="s">
-        <v>74</v>
-      </c>
-      <c r="E32" t="s">
-        <v>57</v>
-      </c>
-      <c r="F32" t="s">
-        <v>178</v>
-      </c>
       <c r="G32">
-        <v>2600000</v>
+        <v>5400000</v>
       </c>
       <c r="H32">
-        <v>0</v>
+        <v>2000000</v>
       </c>
       <c r="I32">
-        <v>280000</v>
+        <v>540000</v>
       </c>
       <c r="J32">
-        <v>380000</v>
+        <v>650000</v>
       </c>
       <c r="K32">
         <v>0</v>
       </c>
       <c r="L32">
-        <v>440000</v>
+        <v>1210000</v>
       </c>
       <c r="M32">
-        <v>0</v>
+        <v>1000000</v>
       </c>
       <c r="N32">
         <v>0</v>
@@ -2832,11 +2801,11 @@
         <v>0</v>
       </c>
       <c r="P32">
-        <v>1800000</v>
+        <v>2900000</v>
       </c>
       <c r="Q32">
-        <f t="shared" si="1"/>
-        <v>5500000</v>
+        <f t="shared" si="0"/>
+        <v>13700000</v>
       </c>
     </row>
     <row r="33" spans="1:17" customFormat="1">
@@ -2845,37 +2814,37 @@
         <v>36</v>
       </c>
       <c r="C33" t="s">
+        <v>178</v>
+      </c>
+      <c r="D33" t="s">
+        <v>73</v>
+      </c>
+      <c r="E33" t="s">
+        <v>52</v>
+      </c>
+      <c r="F33" t="s">
         <v>179</v>
       </c>
-      <c r="D33" t="s">
-        <v>75</v>
-      </c>
-      <c r="E33" t="s">
-        <v>21</v>
-      </c>
-      <c r="F33" t="s">
-        <v>180</v>
-      </c>
       <c r="G33">
-        <v>5400000</v>
+        <v>720000</v>
       </c>
       <c r="H33">
-        <v>2000000</v>
+        <v>210000</v>
       </c>
       <c r="I33">
-        <v>540000</v>
+        <v>38000</v>
       </c>
       <c r="J33">
-        <v>650000</v>
+        <v>330000</v>
       </c>
       <c r="K33">
-        <v>0</v>
+        <v>142000</v>
       </c>
       <c r="L33">
-        <v>1210000</v>
+        <v>0</v>
       </c>
       <c r="M33">
-        <v>1000000</v>
+        <v>0</v>
       </c>
       <c r="N33">
         <v>0</v>
@@ -2884,47 +2853,47 @@
         <v>0</v>
       </c>
       <c r="P33">
-        <v>2900000</v>
+        <v>0</v>
       </c>
       <c r="Q33">
-        <f t="shared" si="1"/>
-        <v>13700000</v>
+        <f t="shared" si="0"/>
+        <v>1440000</v>
       </c>
     </row>
     <row r="34" spans="1:17" customFormat="1">
       <c r="A34" s="4"/>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C34" t="s">
+        <v>180</v>
+      </c>
+      <c r="D34" t="s">
+        <v>74</v>
+      </c>
+      <c r="E34" t="s">
+        <v>21</v>
+      </c>
+      <c r="F34" t="s">
         <v>181</v>
       </c>
-      <c r="D34" t="s">
-        <v>76</v>
-      </c>
-      <c r="E34" t="s">
-        <v>55</v>
-      </c>
-      <c r="F34" t="s">
-        <v>182</v>
-      </c>
       <c r="G34">
-        <v>720000</v>
+        <v>16000000</v>
       </c>
       <c r="H34">
-        <v>210000</v>
+        <v>5800000</v>
       </c>
       <c r="I34">
-        <v>38000</v>
+        <v>1600000</v>
       </c>
       <c r="J34">
-        <v>330000</v>
+        <v>1900000</v>
       </c>
       <c r="K34">
-        <v>142000</v>
+        <v>3500000</v>
       </c>
       <c r="L34">
-        <v>0</v>
+        <v>3200000</v>
       </c>
       <c r="M34">
         <v>0</v>
@@ -2936,11 +2905,11 @@
         <v>0</v>
       </c>
       <c r="P34">
-        <v>0</v>
+        <v>3800000</v>
       </c>
       <c r="Q34">
-        <f t="shared" si="1"/>
-        <v>1440000</v>
+        <f t="shared" si="0"/>
+        <v>35800000</v>
       </c>
     </row>
     <row r="35" spans="1:17" customFormat="1">
@@ -2949,34 +2918,34 @@
         <v>33</v>
       </c>
       <c r="C35" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D35" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E35" t="s">
         <v>21</v>
       </c>
       <c r="F35" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G35">
-        <v>16000000</v>
+        <v>11500000</v>
       </c>
       <c r="H35">
-        <v>5800000</v>
+        <v>4200000</v>
       </c>
       <c r="I35">
-        <v>1600000</v>
+        <v>1150000</v>
       </c>
       <c r="J35">
-        <v>1900000</v>
+        <v>1380000</v>
       </c>
       <c r="K35">
-        <v>3500000</v>
+        <v>2600000</v>
       </c>
       <c r="L35">
-        <v>3200000</v>
+        <v>2170000</v>
       </c>
       <c r="M35">
         <v>0</v>
@@ -2988,11 +2957,11 @@
         <v>0</v>
       </c>
       <c r="P35">
-        <v>3800000</v>
+        <v>2800000</v>
       </c>
       <c r="Q35">
-        <f t="shared" si="1"/>
-        <v>35800000</v>
+        <f t="shared" si="0"/>
+        <v>25800000</v>
       </c>
     </row>
     <row r="36" spans="1:17" customFormat="1">
@@ -3001,34 +2970,34 @@
         <v>33</v>
       </c>
       <c r="C36" t="s">
+        <v>184</v>
+      </c>
+      <c r="D36" t="s">
+        <v>76</v>
+      </c>
+      <c r="E36" t="s">
+        <v>54</v>
+      </c>
+      <c r="F36" t="s">
         <v>185</v>
       </c>
-      <c r="D36" t="s">
-        <v>78</v>
-      </c>
-      <c r="E36" t="s">
-        <v>21</v>
-      </c>
-      <c r="F36" t="s">
-        <v>186</v>
-      </c>
       <c r="G36">
-        <v>11500000</v>
+        <v>3200000</v>
       </c>
       <c r="H36">
-        <v>4200000</v>
+        <v>0</v>
       </c>
       <c r="I36">
-        <v>1150000</v>
+        <v>320000</v>
       </c>
       <c r="J36">
-        <v>1380000</v>
+        <v>460000</v>
       </c>
       <c r="K36">
-        <v>2600000</v>
+        <v>0</v>
       </c>
       <c r="L36">
-        <v>2170000</v>
+        <v>620000</v>
       </c>
       <c r="M36">
         <v>0</v>
@@ -3040,47 +3009,47 @@
         <v>0</v>
       </c>
       <c r="P36">
-        <v>2800000</v>
+        <v>2100000</v>
       </c>
       <c r="Q36">
-        <f t="shared" si="1"/>
-        <v>25800000</v>
+        <f t="shared" si="0"/>
+        <v>6700000</v>
       </c>
     </row>
     <row r="37" spans="1:17" customFormat="1">
       <c r="A37" s="4"/>
       <c r="B37" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C37" t="s">
+        <v>186</v>
+      </c>
+      <c r="D37" t="s">
+        <v>77</v>
+      </c>
+      <c r="E37" t="s">
+        <v>21</v>
+      </c>
+      <c r="F37" t="s">
         <v>187</v>
       </c>
-      <c r="D37" t="s">
-        <v>79</v>
-      </c>
-      <c r="E37" t="s">
-        <v>57</v>
-      </c>
-      <c r="F37" t="s">
-        <v>188</v>
-      </c>
       <c r="G37">
-        <v>3200000</v>
+        <v>6200000</v>
       </c>
       <c r="H37">
-        <v>0</v>
+        <v>2300000</v>
       </c>
       <c r="I37">
-        <v>320000</v>
+        <v>620000</v>
       </c>
       <c r="J37">
-        <v>460000</v>
+        <v>740000</v>
       </c>
       <c r="K37">
-        <v>0</v>
+        <v>1400000</v>
       </c>
       <c r="L37">
-        <v>620000</v>
+        <v>1140000</v>
       </c>
       <c r="M37">
         <v>0</v>
@@ -3092,47 +3061,47 @@
         <v>0</v>
       </c>
       <c r="P37">
-        <v>2100000</v>
+        <v>2500000</v>
       </c>
       <c r="Q37">
-        <f t="shared" si="1"/>
-        <v>6700000</v>
+        <f t="shared" si="0"/>
+        <v>14900000</v>
       </c>
     </row>
     <row r="38" spans="1:17" customFormat="1">
       <c r="A38" s="4"/>
       <c r="B38" t="s">
-        <v>37</v>
+        <v>79</v>
       </c>
       <c r="C38" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D38" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E38" t="s">
         <v>21</v>
       </c>
       <c r="F38" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G38">
-        <v>6200000</v>
+        <v>4800000</v>
       </c>
       <c r="H38">
-        <v>2300000</v>
+        <v>1800000</v>
       </c>
       <c r="I38">
-        <v>620000</v>
+        <v>480000</v>
       </c>
       <c r="J38">
-        <v>740000</v>
+        <v>580000</v>
       </c>
       <c r="K38">
-        <v>1400000</v>
+        <v>1100000</v>
       </c>
       <c r="L38">
-        <v>1140000</v>
+        <v>840000</v>
       </c>
       <c r="M38">
         <v>0</v>
@@ -3144,48 +3113,48 @@
         <v>0</v>
       </c>
       <c r="P38">
-        <v>2500000</v>
+        <v>2200000</v>
       </c>
       <c r="Q38">
-        <f t="shared" si="1"/>
-        <v>14900000</v>
+        <f t="shared" si="0"/>
+        <v>11800000</v>
       </c>
     </row>
     <row r="39" spans="1:17" customFormat="1">
       <c r="A39" s="4"/>
       <c r="B39" t="s">
-        <v>82</v>
+        <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D39" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E39" t="s">
         <v>21</v>
       </c>
       <c r="F39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G39">
-        <v>4800000</v>
+        <v>2900000</v>
       </c>
       <c r="H39">
-        <v>1800000</v>
+        <v>1100000</v>
       </c>
       <c r="I39">
+        <v>290000</v>
+      </c>
+      <c r="J39">
+        <v>350000</v>
+      </c>
+      <c r="K39">
+        <v>680000</v>
+      </c>
+      <c r="L39">
         <v>480000</v>
       </c>
-      <c r="J39">
-        <v>580000</v>
-      </c>
-      <c r="K39">
-        <v>1100000</v>
-      </c>
-      <c r="L39">
-        <v>840000</v>
-      </c>
       <c r="M39">
         <v>0</v>
       </c>
@@ -3196,47 +3165,47 @@
         <v>0</v>
       </c>
       <c r="P39">
-        <v>2200000</v>
+        <v>1600000</v>
       </c>
       <c r="Q39">
-        <f t="shared" si="1"/>
-        <v>11800000</v>
+        <f t="shared" si="0"/>
+        <v>7400000</v>
       </c>
     </row>
     <row r="40" spans="1:17" customFormat="1">
       <c r="A40" s="4"/>
       <c r="B40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D40" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E40" t="s">
         <v>21</v>
       </c>
       <c r="F40" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G40">
-        <v>2900000</v>
+        <v>2400000</v>
       </c>
       <c r="H40">
-        <v>1100000</v>
+        <v>0</v>
       </c>
       <c r="I40">
-        <v>290000</v>
+        <v>240000</v>
       </c>
       <c r="J40">
-        <v>350000</v>
+        <v>340000</v>
       </c>
       <c r="K40">
-        <v>680000</v>
+        <v>0</v>
       </c>
       <c r="L40">
-        <v>480000</v>
+        <v>520000</v>
       </c>
       <c r="M40">
         <v>0</v>
@@ -3248,47 +3217,47 @@
         <v>0</v>
       </c>
       <c r="P40">
-        <v>1600000</v>
+        <v>1900000</v>
       </c>
       <c r="Q40">
-        <f t="shared" si="1"/>
-        <v>7400000</v>
+        <f t="shared" si="0"/>
+        <v>5400000</v>
       </c>
     </row>
     <row r="41" spans="1:17" customFormat="1">
       <c r="A41" s="4"/>
       <c r="B41" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C41" t="s">
+        <v>194</v>
+      </c>
+      <c r="D41" t="s">
+        <v>82</v>
+      </c>
+      <c r="E41" t="s">
+        <v>54</v>
+      </c>
+      <c r="F41" t="s">
         <v>195</v>
       </c>
-      <c r="D41" t="s">
-        <v>84</v>
-      </c>
-      <c r="E41" t="s">
-        <v>21</v>
-      </c>
-      <c r="F41" t="s">
-        <v>196</v>
-      </c>
       <c r="G41">
-        <v>2400000</v>
+        <v>1400000</v>
       </c>
       <c r="H41">
         <v>0</v>
       </c>
       <c r="I41">
-        <v>240000</v>
+        <v>140000</v>
       </c>
       <c r="J41">
-        <v>340000</v>
+        <v>200000</v>
       </c>
       <c r="K41">
         <v>0</v>
       </c>
       <c r="L41">
-        <v>520000</v>
+        <v>260000</v>
       </c>
       <c r="M41">
         <v>0</v>
@@ -3300,47 +3269,47 @@
         <v>0</v>
       </c>
       <c r="P41">
-        <v>1900000</v>
+        <v>980000</v>
       </c>
       <c r="Q41">
-        <f t="shared" si="1"/>
-        <v>5400000</v>
+        <f t="shared" si="0"/>
+        <v>2980000</v>
       </c>
     </row>
     <row r="42" spans="1:17" customFormat="1">
       <c r="A42" s="4"/>
       <c r="B42" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C42" t="s">
+        <v>196</v>
+      </c>
+      <c r="D42" t="s">
+        <v>83</v>
+      </c>
+      <c r="E42" t="s">
+        <v>54</v>
+      </c>
+      <c r="F42" t="s">
         <v>197</v>
       </c>
-      <c r="D42" t="s">
-        <v>85</v>
-      </c>
-      <c r="E42" t="s">
-        <v>57</v>
-      </c>
-      <c r="F42" t="s">
-        <v>198</v>
-      </c>
       <c r="G42">
-        <v>1400000</v>
+        <v>1600000</v>
       </c>
       <c r="H42">
         <v>0</v>
       </c>
       <c r="I42">
-        <v>140000</v>
+        <v>160000</v>
       </c>
       <c r="J42">
-        <v>200000</v>
+        <v>230000</v>
       </c>
       <c r="K42">
         <v>0</v>
       </c>
       <c r="L42">
-        <v>260000</v>
+        <v>310000</v>
       </c>
       <c r="M42">
         <v>0</v>
@@ -3352,47 +3321,47 @@
         <v>0</v>
       </c>
       <c r="P42">
-        <v>980000</v>
+        <v>1100000</v>
       </c>
       <c r="Q42">
-        <f t="shared" si="1"/>
-        <v>2980000</v>
+        <f t="shared" si="0"/>
+        <v>3400000</v>
       </c>
     </row>
     <row r="43" spans="1:17" customFormat="1">
       <c r="A43" s="4"/>
       <c r="B43" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="C43" t="s">
+        <v>198</v>
+      </c>
+      <c r="D43" t="s">
+        <v>84</v>
+      </c>
+      <c r="E43" t="s">
+        <v>54</v>
+      </c>
+      <c r="F43" t="s">
         <v>199</v>
       </c>
-      <c r="D43" t="s">
-        <v>86</v>
-      </c>
-      <c r="E43" t="s">
-        <v>57</v>
-      </c>
-      <c r="F43" t="s">
-        <v>200</v>
-      </c>
       <c r="G43">
-        <v>1600000</v>
+        <v>1200000</v>
       </c>
       <c r="H43">
         <v>0</v>
       </c>
       <c r="I43">
-        <v>160000</v>
+        <v>120000</v>
       </c>
       <c r="J43">
-        <v>230000</v>
+        <v>180000</v>
       </c>
       <c r="K43">
         <v>0</v>
       </c>
       <c r="L43">
-        <v>310000</v>
+        <v>220000</v>
       </c>
       <c r="M43">
         <v>0</v>
@@ -3404,47 +3373,47 @@
         <v>0</v>
       </c>
       <c r="P43">
-        <v>1100000</v>
+        <v>850000</v>
       </c>
       <c r="Q43">
-        <f t="shared" si="1"/>
-        <v>3400000</v>
+        <f t="shared" si="0"/>
+        <v>2570000</v>
       </c>
     </row>
     <row r="44" spans="1:17" customFormat="1">
       <c r="A44" s="4"/>
       <c r="B44" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C44" t="s">
+        <v>200</v>
+      </c>
+      <c r="D44" t="s">
+        <v>86</v>
+      </c>
+      <c r="E44" t="s">
+        <v>54</v>
+      </c>
+      <c r="F44" t="s">
         <v>201</v>
       </c>
-      <c r="D44" t="s">
-        <v>87</v>
-      </c>
-      <c r="E44" t="s">
-        <v>57</v>
-      </c>
-      <c r="F44" t="s">
-        <v>202</v>
-      </c>
       <c r="G44">
-        <v>1200000</v>
+        <v>1050000</v>
       </c>
       <c r="H44">
         <v>0</v>
       </c>
       <c r="I44">
-        <v>120000</v>
+        <v>105000</v>
       </c>
       <c r="J44">
-        <v>180000</v>
+        <v>160000</v>
       </c>
       <c r="K44">
         <v>0</v>
       </c>
       <c r="L44">
-        <v>220000</v>
+        <v>185000</v>
       </c>
       <c r="M44">
         <v>0</v>
@@ -3456,47 +3425,47 @@
         <v>0</v>
       </c>
       <c r="P44">
-        <v>850000</v>
+        <v>750000</v>
       </c>
       <c r="Q44">
-        <f t="shared" si="1"/>
-        <v>2570000</v>
+        <f t="shared" si="0"/>
+        <v>2250000</v>
       </c>
     </row>
     <row r="45" spans="1:17" customFormat="1">
       <c r="A45" s="4"/>
       <c r="B45" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C45" t="s">
+        <v>202</v>
+      </c>
+      <c r="D45" t="s">
+        <v>88</v>
+      </c>
+      <c r="E45" t="s">
+        <v>54</v>
+      </c>
+      <c r="F45" t="s">
         <v>203</v>
       </c>
-      <c r="D45" t="s">
-        <v>89</v>
-      </c>
-      <c r="E45" t="s">
-        <v>57</v>
-      </c>
-      <c r="F45" t="s">
-        <v>204</v>
-      </c>
       <c r="G45">
-        <v>1050000</v>
+        <v>890000</v>
       </c>
       <c r="H45">
         <v>0</v>
       </c>
       <c r="I45">
-        <v>105000</v>
+        <v>89000</v>
       </c>
       <c r="J45">
-        <v>160000</v>
+        <v>135000</v>
       </c>
       <c r="K45">
         <v>0</v>
       </c>
       <c r="L45">
-        <v>185000</v>
+        <v>166000</v>
       </c>
       <c r="M45">
         <v>0</v>
@@ -3508,50 +3477,50 @@
         <v>0</v>
       </c>
       <c r="P45">
-        <v>750000</v>
+        <v>650000</v>
       </c>
       <c r="Q45">
-        <f t="shared" si="1"/>
-        <v>2250000</v>
+        <f t="shared" si="0"/>
+        <v>1930000</v>
       </c>
     </row>
     <row r="46" spans="1:17" customFormat="1">
       <c r="A46" s="4"/>
       <c r="B46" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C46" t="s">
+        <v>204</v>
+      </c>
+      <c r="D46" t="s">
+        <v>90</v>
+      </c>
+      <c r="E46" t="s">
+        <v>21</v>
+      </c>
+      <c r="F46" t="s">
         <v>205</v>
       </c>
-      <c r="D46" t="s">
-        <v>91</v>
-      </c>
-      <c r="E46" t="s">
-        <v>57</v>
-      </c>
-      <c r="F46" t="s">
-        <v>206</v>
-      </c>
       <c r="G46">
-        <v>890000</v>
+        <v>2800000</v>
       </c>
       <c r="H46">
-        <v>0</v>
+        <v>1050000</v>
       </c>
       <c r="I46">
-        <v>89000</v>
+        <v>280000</v>
       </c>
       <c r="J46">
-        <v>135000</v>
+        <v>340000</v>
       </c>
       <c r="K46">
         <v>0</v>
       </c>
       <c r="L46">
-        <v>166000</v>
+        <v>630000</v>
       </c>
       <c r="M46">
-        <v>0</v>
+        <v>500000</v>
       </c>
       <c r="N46">
         <v>0</v>
@@ -3560,50 +3529,50 @@
         <v>0</v>
       </c>
       <c r="P46">
-        <v>650000</v>
+        <v>1800000</v>
       </c>
       <c r="Q46">
-        <f t="shared" si="1"/>
-        <v>1930000</v>
+        <f t="shared" si="0"/>
+        <v>7400000</v>
       </c>
     </row>
     <row r="47" spans="1:17" customFormat="1">
       <c r="A47" s="4"/>
       <c r="B47" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C47" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D47" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E47" t="s">
         <v>21</v>
       </c>
       <c r="F47" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G47">
-        <v>2800000</v>
+        <v>2100000</v>
       </c>
       <c r="H47">
-        <v>1050000</v>
+        <v>780000</v>
       </c>
       <c r="I47">
-        <v>280000</v>
+        <v>210000</v>
       </c>
       <c r="J47">
+        <v>250000</v>
+      </c>
+      <c r="K47">
+        <v>520000</v>
+      </c>
+      <c r="L47">
         <v>340000</v>
       </c>
-      <c r="K47">
-        <v>0</v>
-      </c>
-      <c r="L47">
-        <v>630000</v>
-      </c>
       <c r="M47">
-        <v>500000</v>
+        <v>0</v>
       </c>
       <c r="N47">
         <v>0</v>
@@ -3612,47 +3581,47 @@
         <v>0</v>
       </c>
       <c r="P47">
-        <v>1800000</v>
+        <v>1200000</v>
       </c>
       <c r="Q47">
-        <f t="shared" si="1"/>
-        <v>7400000</v>
+        <f t="shared" si="0"/>
+        <v>5400000</v>
       </c>
     </row>
     <row r="48" spans="1:17" customFormat="1">
       <c r="A48" s="4"/>
       <c r="B48" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C48" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D48" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E48" t="s">
         <v>21</v>
       </c>
       <c r="F48" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G48">
-        <v>2100000</v>
+        <v>4500000</v>
       </c>
       <c r="H48">
-        <v>780000</v>
+        <v>1650000</v>
       </c>
       <c r="I48">
-        <v>210000</v>
+        <v>450000</v>
       </c>
       <c r="J48">
-        <v>250000</v>
+        <v>540000</v>
       </c>
       <c r="K48">
-        <v>520000</v>
+        <v>1050000</v>
       </c>
       <c r="L48">
-        <v>340000</v>
+        <v>810000</v>
       </c>
       <c r="M48">
         <v>0</v>
@@ -3664,47 +3633,47 @@
         <v>0</v>
       </c>
       <c r="P48">
-        <v>1200000</v>
+        <v>1900000</v>
       </c>
       <c r="Q48">
-        <f t="shared" si="1"/>
-        <v>5400000</v>
+        <f t="shared" si="0"/>
+        <v>10900000</v>
       </c>
     </row>
     <row r="49" spans="1:17" customFormat="1">
       <c r="A49" s="4"/>
       <c r="B49" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C49" t="s">
+        <v>210</v>
+      </c>
+      <c r="D49" t="s">
+        <v>96</v>
+      </c>
+      <c r="E49" t="s">
+        <v>54</v>
+      </c>
+      <c r="F49" t="s">
         <v>211</v>
       </c>
-      <c r="D49" t="s">
-        <v>97</v>
-      </c>
-      <c r="E49" t="s">
-        <v>21</v>
-      </c>
-      <c r="F49" t="s">
-        <v>212</v>
-      </c>
       <c r="G49">
-        <v>4500000</v>
+        <v>1150000</v>
       </c>
       <c r="H49">
-        <v>1650000</v>
+        <v>0</v>
       </c>
       <c r="I49">
-        <v>450000</v>
+        <v>115000</v>
       </c>
       <c r="J49">
-        <v>540000</v>
+        <v>175000</v>
       </c>
       <c r="K49">
-        <v>1050000</v>
+        <v>0</v>
       </c>
       <c r="L49">
-        <v>810000</v>
+        <v>210000</v>
       </c>
       <c r="M49">
         <v>0</v>
@@ -3716,47 +3685,47 @@
         <v>0</v>
       </c>
       <c r="P49">
-        <v>1900000</v>
+        <v>800000</v>
       </c>
       <c r="Q49">
-        <f t="shared" si="1"/>
-        <v>10900000</v>
+        <f t="shared" si="0"/>
+        <v>2450000</v>
       </c>
     </row>
     <row r="50" spans="1:17" customFormat="1">
       <c r="A50" s="4"/>
       <c r="B50" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C50" t="s">
+        <v>212</v>
+      </c>
+      <c r="D50" t="s">
+        <v>98</v>
+      </c>
+      <c r="E50" t="s">
+        <v>52</v>
+      </c>
+      <c r="F50" t="s">
         <v>213</v>
       </c>
-      <c r="D50" t="s">
-        <v>99</v>
-      </c>
-      <c r="E50" t="s">
-        <v>57</v>
-      </c>
-      <c r="F50" t="s">
-        <v>214</v>
-      </c>
       <c r="G50">
-        <v>1150000</v>
+        <v>580000</v>
       </c>
       <c r="H50">
-        <v>0</v>
+        <v>170000</v>
       </c>
       <c r="I50">
+        <v>30000</v>
+      </c>
+      <c r="J50">
+        <v>265000</v>
+      </c>
+      <c r="K50">
         <v>115000</v>
       </c>
-      <c r="J50">
-        <v>175000</v>
-      </c>
-      <c r="K50">
-        <v>0</v>
-      </c>
       <c r="L50">
-        <v>210000</v>
+        <v>0</v>
       </c>
       <c r="M50">
         <v>0</v>
@@ -3768,47 +3737,47 @@
         <v>0</v>
       </c>
       <c r="P50">
-        <v>800000</v>
+        <v>0</v>
       </c>
       <c r="Q50">
-        <f t="shared" si="1"/>
-        <v>2450000</v>
+        <f t="shared" si="0"/>
+        <v>1160000</v>
       </c>
     </row>
     <row r="51" spans="1:17" customFormat="1">
       <c r="A51" s="4"/>
       <c r="B51" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C51" t="s">
+        <v>214</v>
+      </c>
+      <c r="D51" t="s">
+        <v>100</v>
+      </c>
+      <c r="E51" t="s">
+        <v>21</v>
+      </c>
+      <c r="F51" t="s">
         <v>215</v>
       </c>
-      <c r="D51" t="s">
-        <v>101</v>
-      </c>
-      <c r="E51" t="s">
-        <v>55</v>
-      </c>
-      <c r="F51" t="s">
-        <v>216</v>
-      </c>
       <c r="G51">
-        <v>580000</v>
+        <v>5200000</v>
       </c>
       <c r="H51">
-        <v>170000</v>
+        <v>1900000</v>
       </c>
       <c r="I51">
-        <v>30000</v>
+        <v>520000</v>
       </c>
       <c r="J51">
-        <v>265000</v>
+        <v>620000</v>
       </c>
       <c r="K51">
-        <v>115000</v>
+        <v>1200000</v>
       </c>
       <c r="L51">
-        <v>0</v>
+        <v>960000</v>
       </c>
       <c r="M51">
         <v>0</v>
@@ -3820,47 +3789,47 @@
         <v>0</v>
       </c>
       <c r="P51">
-        <v>0</v>
+        <v>2400000</v>
       </c>
       <c r="Q51">
-        <f t="shared" si="1"/>
-        <v>1160000</v>
+        <f t="shared" si="0"/>
+        <v>12800000</v>
       </c>
     </row>
     <row r="52" spans="1:17" customFormat="1">
       <c r="A52" s="4"/>
       <c r="B52" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C52" t="s">
+        <v>216</v>
+      </c>
+      <c r="D52" t="s">
+        <v>102</v>
+      </c>
+      <c r="E52" t="s">
+        <v>54</v>
+      </c>
+      <c r="F52" t="s">
         <v>217</v>
       </c>
-      <c r="D52" t="s">
-        <v>103</v>
-      </c>
-      <c r="E52" t="s">
-        <v>21</v>
-      </c>
-      <c r="F52" t="s">
-        <v>218</v>
-      </c>
       <c r="G52">
-        <v>5200000</v>
+        <v>1400000</v>
       </c>
       <c r="H52">
-        <v>1900000</v>
+        <v>0</v>
       </c>
       <c r="I52">
-        <v>520000</v>
+        <v>140000</v>
       </c>
       <c r="J52">
-        <v>620000</v>
+        <v>200000</v>
       </c>
       <c r="K52">
-        <v>1200000</v>
+        <v>0</v>
       </c>
       <c r="L52">
-        <v>960000</v>
+        <v>260000</v>
       </c>
       <c r="M52">
         <v>0</v>
@@ -3872,47 +3841,47 @@
         <v>0</v>
       </c>
       <c r="P52">
-        <v>2400000</v>
+        <v>950000</v>
       </c>
       <c r="Q52">
-        <f t="shared" si="1"/>
-        <v>12800000</v>
+        <f t="shared" si="0"/>
+        <v>2950000</v>
       </c>
     </row>
     <row r="53" spans="1:17" customFormat="1">
       <c r="A53" s="4"/>
       <c r="B53" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C53" t="s">
+        <v>218</v>
+      </c>
+      <c r="D53" t="s">
+        <v>104</v>
+      </c>
+      <c r="E53" t="s">
+        <v>54</v>
+      </c>
+      <c r="F53" t="s">
         <v>219</v>
       </c>
-      <c r="D53" t="s">
-        <v>105</v>
-      </c>
-      <c r="E53" t="s">
-        <v>57</v>
-      </c>
-      <c r="F53" t="s">
-        <v>220</v>
-      </c>
       <c r="G53">
-        <v>1400000</v>
+        <v>1080000</v>
       </c>
       <c r="H53">
         <v>0</v>
       </c>
       <c r="I53">
-        <v>140000</v>
+        <v>108000</v>
       </c>
       <c r="J53">
-        <v>200000</v>
+        <v>165000</v>
       </c>
       <c r="K53">
         <v>0</v>
       </c>
       <c r="L53">
-        <v>260000</v>
+        <v>197000</v>
       </c>
       <c r="M53">
         <v>0</v>
@@ -3924,47 +3893,47 @@
         <v>0</v>
       </c>
       <c r="P53">
-        <v>950000</v>
+        <v>750000</v>
       </c>
       <c r="Q53">
-        <f t="shared" si="1"/>
-        <v>2950000</v>
+        <f t="shared" si="0"/>
+        <v>2300000</v>
       </c>
     </row>
     <row r="54" spans="1:17" customFormat="1">
       <c r="A54" s="4"/>
       <c r="B54" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C54" t="s">
+        <v>220</v>
+      </c>
+      <c r="D54" t="s">
+        <v>106</v>
+      </c>
+      <c r="E54" t="s">
+        <v>54</v>
+      </c>
+      <c r="F54" t="s">
         <v>221</v>
       </c>
-      <c r="D54" t="s">
-        <v>107</v>
-      </c>
-      <c r="E54" t="s">
-        <v>57</v>
-      </c>
-      <c r="F54" t="s">
-        <v>222</v>
-      </c>
       <c r="G54">
-        <v>1080000</v>
+        <v>920000</v>
       </c>
       <c r="H54">
         <v>0</v>
       </c>
       <c r="I54">
-        <v>108000</v>
+        <v>92000</v>
       </c>
       <c r="J54">
-        <v>165000</v>
+        <v>140000</v>
       </c>
       <c r="K54">
         <v>0</v>
       </c>
       <c r="L54">
-        <v>197000</v>
+        <v>168000</v>
       </c>
       <c r="M54">
         <v>0</v>
@@ -3976,47 +3945,47 @@
         <v>0</v>
       </c>
       <c r="P54">
-        <v>750000</v>
+        <v>650000</v>
       </c>
       <c r="Q54">
-        <f t="shared" si="1"/>
-        <v>2300000</v>
+        <f t="shared" si="0"/>
+        <v>1970000</v>
       </c>
     </row>
     <row r="55" spans="1:17" customFormat="1">
       <c r="A55" s="4"/>
       <c r="B55" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="C55" t="s">
+        <v>222</v>
+      </c>
+      <c r="D55" t="s">
+        <v>108</v>
+      </c>
+      <c r="E55" t="s">
+        <v>21</v>
+      </c>
+      <c r="F55" t="s">
         <v>223</v>
       </c>
-      <c r="D55" t="s">
-        <v>109</v>
-      </c>
-      <c r="E55" t="s">
-        <v>57</v>
-      </c>
-      <c r="F55" t="s">
-        <v>224</v>
-      </c>
       <c r="G55">
-        <v>920000</v>
+        <v>3300000</v>
       </c>
       <c r="H55">
-        <v>0</v>
+        <v>1200000</v>
       </c>
       <c r="I55">
-        <v>92000</v>
+        <v>330000</v>
       </c>
       <c r="J55">
-        <v>140000</v>
+        <v>390000</v>
       </c>
       <c r="K55">
-        <v>0</v>
+        <v>780000</v>
       </c>
       <c r="L55">
-        <v>168000</v>
+        <v>600000</v>
       </c>
       <c r="M55">
         <v>0</v>
@@ -4028,47 +3997,47 @@
         <v>0</v>
       </c>
       <c r="P55">
-        <v>650000</v>
+        <v>1900000</v>
       </c>
       <c r="Q55">
-        <f t="shared" si="1"/>
-        <v>1970000</v>
+        <f t="shared" si="0"/>
+        <v>8500000</v>
       </c>
     </row>
     <row r="56" spans="1:17" customFormat="1">
       <c r="A56" s="4"/>
       <c r="B56" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="C56" t="s">
+        <v>224</v>
+      </c>
+      <c r="D56" t="s">
+        <v>109</v>
+      </c>
+      <c r="E56" t="s">
+        <v>52</v>
+      </c>
+      <c r="F56" t="s">
         <v>225</v>
       </c>
-      <c r="D56" t="s">
-        <v>111</v>
-      </c>
-      <c r="E56" t="s">
-        <v>21</v>
-      </c>
-      <c r="F56" t="s">
-        <v>226</v>
-      </c>
       <c r="G56">
-        <v>3300000</v>
+        <v>780000</v>
       </c>
       <c r="H56">
-        <v>1200000</v>
+        <v>230000</v>
       </c>
       <c r="I56">
-        <v>330000</v>
+        <v>40000</v>
       </c>
       <c r="J56">
-        <v>390000</v>
+        <v>360000</v>
       </c>
       <c r="K56">
-        <v>780000</v>
+        <v>150000</v>
       </c>
       <c r="L56">
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="M56">
         <v>0</v>
@@ -4080,44 +4049,44 @@
         <v>0</v>
       </c>
       <c r="P56">
-        <v>1900000</v>
+        <v>0</v>
       </c>
       <c r="Q56">
-        <f t="shared" si="1"/>
-        <v>8500000</v>
+        <f t="shared" si="0"/>
+        <v>1560000</v>
       </c>
     </row>
     <row r="57" spans="1:17" customFormat="1">
       <c r="A57" s="4"/>
       <c r="B57" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C57" t="s">
+        <v>226</v>
+      </c>
+      <c r="D57" t="s">
+        <v>110</v>
+      </c>
+      <c r="E57" t="s">
+        <v>52</v>
+      </c>
+      <c r="F57" t="s">
         <v>227</v>
       </c>
-      <c r="D57" t="s">
-        <v>112</v>
-      </c>
-      <c r="E57" t="s">
-        <v>55</v>
-      </c>
-      <c r="F57" t="s">
-        <v>228</v>
-      </c>
       <c r="G57">
-        <v>780000</v>
+        <v>980000</v>
       </c>
       <c r="H57">
-        <v>230000</v>
+        <v>290000</v>
       </c>
       <c r="I57">
-        <v>40000</v>
+        <v>48000</v>
       </c>
       <c r="J57">
-        <v>360000</v>
+        <v>450000</v>
       </c>
       <c r="K57">
-        <v>150000</v>
+        <v>192000</v>
       </c>
       <c r="L57">
         <v>0</v>
@@ -4135,41 +4104,41 @@
         <v>0</v>
       </c>
       <c r="Q57">
-        <f t="shared" si="1"/>
-        <v>1560000</v>
+        <f t="shared" si="0"/>
+        <v>1960000</v>
       </c>
     </row>
     <row r="58" spans="1:17" customFormat="1">
       <c r="A58" s="4"/>
       <c r="B58" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C58" t="s">
+        <v>228</v>
+      </c>
+      <c r="D58" t="s">
+        <v>111</v>
+      </c>
+      <c r="E58" t="s">
+        <v>52</v>
+      </c>
+      <c r="F58" t="s">
         <v>229</v>
       </c>
-      <c r="D58" t="s">
-        <v>113</v>
-      </c>
-      <c r="E58" t="s">
-        <v>55</v>
-      </c>
-      <c r="F58" t="s">
-        <v>230</v>
-      </c>
       <c r="G58">
-        <v>980000</v>
+        <v>620000</v>
       </c>
       <c r="H58">
-        <v>290000</v>
+        <v>180000</v>
       </c>
       <c r="I58">
-        <v>48000</v>
+        <v>32000</v>
       </c>
       <c r="J58">
-        <v>450000</v>
+        <v>285000</v>
       </c>
       <c r="K58">
-        <v>192000</v>
+        <v>123000</v>
       </c>
       <c r="L58">
         <v>0</v>
@@ -4187,41 +4156,41 @@
         <v>0</v>
       </c>
       <c r="Q58">
-        <f t="shared" si="1"/>
-        <v>1960000</v>
+        <f t="shared" si="0"/>
+        <v>1240000</v>
       </c>
     </row>
     <row r="59" spans="1:17" customFormat="1">
       <c r="A59" s="4"/>
       <c r="B59" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C59" t="s">
+        <v>230</v>
+      </c>
+      <c r="D59" t="s">
+        <v>112</v>
+      </c>
+      <c r="E59" t="s">
+        <v>52</v>
+      </c>
+      <c r="F59" t="s">
         <v>231</v>
       </c>
-      <c r="D59" t="s">
-        <v>114</v>
-      </c>
-      <c r="E59" t="s">
-        <v>55</v>
-      </c>
-      <c r="F59" t="s">
-        <v>232</v>
-      </c>
       <c r="G59">
-        <v>620000</v>
+        <v>850000</v>
       </c>
       <c r="H59">
-        <v>180000</v>
+        <v>250000</v>
       </c>
       <c r="I59">
-        <v>32000</v>
+        <v>42000</v>
       </c>
       <c r="J59">
-        <v>285000</v>
+        <v>390000</v>
       </c>
       <c r="K59">
-        <v>123000</v>
+        <v>168000</v>
       </c>
       <c r="L59">
         <v>0</v>
@@ -4239,41 +4208,41 @@
         <v>0</v>
       </c>
       <c r="Q59">
-        <f t="shared" si="1"/>
-        <v>1240000</v>
+        <f t="shared" si="0"/>
+        <v>1700000</v>
       </c>
     </row>
     <row r="60" spans="1:17" customFormat="1">
       <c r="A60" s="4"/>
       <c r="B60" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="C60" t="s">
+        <v>232</v>
+      </c>
+      <c r="D60" t="s">
+        <v>113</v>
+      </c>
+      <c r="E60" t="s">
+        <v>52</v>
+      </c>
+      <c r="F60" t="s">
         <v>233</v>
       </c>
-      <c r="D60" t="s">
-        <v>115</v>
-      </c>
-      <c r="E60" t="s">
-        <v>55</v>
-      </c>
-      <c r="F60" t="s">
-        <v>234</v>
-      </c>
       <c r="G60">
-        <v>850000</v>
+        <v>690000</v>
       </c>
       <c r="H60">
-        <v>250000</v>
+        <v>200000</v>
       </c>
       <c r="I60">
-        <v>42000</v>
+        <v>35000</v>
       </c>
       <c r="J60">
-        <v>390000</v>
+        <v>315000</v>
       </c>
       <c r="K60">
-        <v>168000</v>
+        <v>140000</v>
       </c>
       <c r="L60">
         <v>0</v>
@@ -4291,41 +4260,41 @@
         <v>0</v>
       </c>
       <c r="Q60">
-        <f t="shared" si="1"/>
-        <v>1700000</v>
+        <f t="shared" si="0"/>
+        <v>1380000</v>
       </c>
     </row>
     <row r="61" spans="1:17" customFormat="1">
       <c r="A61" s="4"/>
       <c r="B61" t="s">
-        <v>29</v>
+        <v>115</v>
       </c>
       <c r="C61" t="s">
+        <v>234</v>
+      </c>
+      <c r="D61" t="s">
+        <v>114</v>
+      </c>
+      <c r="E61" t="s">
+        <v>52</v>
+      </c>
+      <c r="F61" t="s">
         <v>235</v>
       </c>
-      <c r="D61" t="s">
-        <v>116</v>
-      </c>
-      <c r="E61" t="s">
-        <v>55</v>
-      </c>
-      <c r="F61" t="s">
-        <v>236</v>
-      </c>
       <c r="G61">
-        <v>690000</v>
+        <v>480000</v>
       </c>
       <c r="H61">
-        <v>200000</v>
+        <v>140000</v>
       </c>
       <c r="I61">
-        <v>35000</v>
+        <v>25000</v>
       </c>
       <c r="J61">
-        <v>315000</v>
+        <v>220000</v>
       </c>
       <c r="K61">
-        <v>140000</v>
+        <v>95000</v>
       </c>
       <c r="L61">
         <v>0</v>
@@ -4343,41 +4312,41 @@
         <v>0</v>
       </c>
       <c r="Q61">
-        <f t="shared" si="1"/>
-        <v>1380000</v>
+        <f t="shared" si="0"/>
+        <v>960000</v>
       </c>
     </row>
     <row r="62" spans="1:17" customFormat="1">
       <c r="A62" s="4"/>
       <c r="B62" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C62" t="s">
+        <v>236</v>
+      </c>
+      <c r="D62" t="s">
+        <v>116</v>
+      </c>
+      <c r="E62" t="s">
+        <v>52</v>
+      </c>
+      <c r="F62" t="s">
         <v>237</v>
       </c>
-      <c r="D62" t="s">
-        <v>117</v>
-      </c>
-      <c r="E62" t="s">
-        <v>55</v>
-      </c>
-      <c r="F62" t="s">
-        <v>238</v>
-      </c>
       <c r="G62">
-        <v>480000</v>
+        <v>520000</v>
       </c>
       <c r="H62">
-        <v>140000</v>
+        <v>152000</v>
       </c>
       <c r="I62">
-        <v>25000</v>
+        <v>27000</v>
       </c>
       <c r="J62">
-        <v>220000</v>
+        <v>238000</v>
       </c>
       <c r="K62">
-        <v>95000</v>
+        <v>103000</v>
       </c>
       <c r="L62">
         <v>0</v>
@@ -4395,41 +4364,41 @@
         <v>0</v>
       </c>
       <c r="Q62">
-        <f t="shared" si="1"/>
-        <v>960000</v>
+        <f t="shared" si="0"/>
+        <v>1040000</v>
       </c>
     </row>
     <row r="63" spans="1:17" customFormat="1">
       <c r="A63" s="4"/>
       <c r="B63" t="s">
-        <v>120</v>
+        <v>93</v>
       </c>
       <c r="C63" t="s">
+        <v>238</v>
+      </c>
+      <c r="D63" t="s">
+        <v>118</v>
+      </c>
+      <c r="E63" t="s">
+        <v>52</v>
+      </c>
+      <c r="F63" t="s">
         <v>239</v>
       </c>
-      <c r="D63" t="s">
-        <v>119</v>
-      </c>
-      <c r="E63" t="s">
-        <v>55</v>
-      </c>
-      <c r="F63" t="s">
-        <v>240</v>
-      </c>
       <c r="G63">
-        <v>520000</v>
+        <v>420000</v>
       </c>
       <c r="H63">
-        <v>152000</v>
+        <v>122000</v>
       </c>
       <c r="I63">
-        <v>27000</v>
+        <v>22000</v>
       </c>
       <c r="J63">
-        <v>238000</v>
+        <v>192000</v>
       </c>
       <c r="K63">
-        <v>103000</v>
+        <v>84000</v>
       </c>
       <c r="L63">
         <v>0</v>
@@ -4447,41 +4416,41 @@
         <v>0</v>
       </c>
       <c r="Q63">
-        <f t="shared" si="1"/>
-        <v>1040000</v>
+        <f t="shared" si="0"/>
+        <v>840000</v>
       </c>
     </row>
     <row r="64" spans="1:17" customFormat="1">
       <c r="A64" s="4"/>
       <c r="B64" t="s">
-        <v>96</v>
+        <v>37</v>
       </c>
       <c r="C64" t="s">
+        <v>240</v>
+      </c>
+      <c r="D64" t="s">
+        <v>119</v>
+      </c>
+      <c r="E64" t="s">
+        <v>52</v>
+      </c>
+      <c r="F64" t="s">
         <v>241</v>
       </c>
-      <c r="D64" t="s">
-        <v>121</v>
-      </c>
-      <c r="E64" t="s">
-        <v>55</v>
-      </c>
-      <c r="F64" t="s">
-        <v>242</v>
-      </c>
       <c r="G64">
-        <v>420000</v>
+        <v>580000</v>
       </c>
       <c r="H64">
-        <v>122000</v>
+        <v>170000</v>
       </c>
       <c r="I64">
-        <v>22000</v>
+        <v>30000</v>
       </c>
       <c r="J64">
-        <v>192000</v>
+        <v>265000</v>
       </c>
       <c r="K64">
-        <v>84000</v>
+        <v>115000</v>
       </c>
       <c r="L64">
         <v>0</v>
@@ -4499,44 +4468,44 @@
         <v>0</v>
       </c>
       <c r="Q64">
-        <f t="shared" si="1"/>
-        <v>840000</v>
+        <f t="shared" si="0"/>
+        <v>1160000</v>
       </c>
     </row>
     <row r="65" spans="1:47" customFormat="1">
       <c r="A65" s="4"/>
       <c r="B65" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C65" t="s">
+        <v>242</v>
+      </c>
+      <c r="D65" t="s">
+        <v>120</v>
+      </c>
+      <c r="E65" t="s">
+        <v>54</v>
+      </c>
+      <c r="F65" t="s">
         <v>243</v>
       </c>
-      <c r="D65" t="s">
-        <v>122</v>
-      </c>
-      <c r="E65" t="s">
-        <v>55</v>
-      </c>
-      <c r="F65" t="s">
-        <v>244</v>
-      </c>
       <c r="G65">
-        <v>580000</v>
+        <v>680000</v>
       </c>
       <c r="H65">
-        <v>170000</v>
+        <v>0</v>
       </c>
       <c r="I65">
-        <v>30000</v>
+        <v>68000</v>
       </c>
       <c r="J65">
-        <v>265000</v>
+        <v>105000</v>
       </c>
       <c r="K65">
-        <v>115000</v>
+        <v>0</v>
       </c>
       <c r="L65">
-        <v>0</v>
+        <v>127000</v>
       </c>
       <c r="M65">
         <v>0</v>
@@ -4548,47 +4517,47 @@
         <v>0</v>
       </c>
       <c r="P65">
-        <v>0</v>
+        <v>520000</v>
       </c>
       <c r="Q65">
-        <f t="shared" si="1"/>
-        <v>1160000</v>
+        <f t="shared" si="0"/>
+        <v>1500000</v>
       </c>
     </row>
     <row r="66" spans="1:47" customFormat="1">
       <c r="A66" s="4"/>
       <c r="B66" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C66" t="s">
+        <v>244</v>
+      </c>
+      <c r="D66" t="s">
+        <v>121</v>
+      </c>
+      <c r="E66" t="s">
+        <v>54</v>
+      </c>
+      <c r="F66" t="s">
         <v>245</v>
       </c>
-      <c r="D66" t="s">
-        <v>123</v>
-      </c>
-      <c r="E66" t="s">
-        <v>57</v>
-      </c>
-      <c r="F66" t="s">
-        <v>246</v>
-      </c>
       <c r="G66">
-        <v>680000</v>
+        <v>2800000</v>
       </c>
       <c r="H66">
         <v>0</v>
       </c>
       <c r="I66">
-        <v>68000</v>
+        <v>280000</v>
       </c>
       <c r="J66">
-        <v>105000</v>
+        <v>410000</v>
       </c>
       <c r="K66">
         <v>0</v>
       </c>
       <c r="L66">
-        <v>127000</v>
+        <v>530000</v>
       </c>
       <c r="M66">
         <v>0</v>
@@ -4600,11 +4569,11 @@
         <v>0</v>
       </c>
       <c r="P66">
-        <v>520000</v>
+        <v>1900000</v>
       </c>
       <c r="Q66">
-        <f t="shared" si="1"/>
-        <v>1500000</v>
+        <f t="shared" si="0"/>
+        <v>5920000</v>
       </c>
     </row>
     <row r="67" spans="1:47" customFormat="1">
@@ -4613,34 +4582,34 @@
         <v>34</v>
       </c>
       <c r="C67" t="s">
+        <v>246</v>
+      </c>
+      <c r="D67" t="s">
+        <v>122</v>
+      </c>
+      <c r="E67" t="s">
+        <v>54</v>
+      </c>
+      <c r="F67" t="s">
         <v>247</v>
       </c>
-      <c r="D67" t="s">
-        <v>124</v>
-      </c>
-      <c r="E67" t="s">
-        <v>57</v>
-      </c>
-      <c r="F67" t="s">
-        <v>248</v>
-      </c>
       <c r="G67">
-        <v>2800000</v>
+        <v>2200000</v>
       </c>
       <c r="H67">
         <v>0</v>
       </c>
       <c r="I67">
-        <v>280000</v>
+        <v>220000</v>
       </c>
       <c r="J67">
-        <v>410000</v>
+        <v>320000</v>
       </c>
       <c r="K67">
         <v>0</v>
       </c>
       <c r="L67">
-        <v>530000</v>
+        <v>440000</v>
       </c>
       <c r="M67">
         <v>0</v>
@@ -4652,11 +4621,11 @@
         <v>0</v>
       </c>
       <c r="P67">
-        <v>1900000</v>
+        <v>1500000</v>
       </c>
       <c r="Q67">
-        <f t="shared" si="1"/>
-        <v>5920000</v>
+        <f t="shared" si="0"/>
+        <v>4680000</v>
       </c>
     </row>
     <row r="68" spans="1:47" customFormat="1">
@@ -4665,34 +4634,34 @@
         <v>34</v>
       </c>
       <c r="C68" t="s">
+        <v>248</v>
+      </c>
+      <c r="D68" t="s">
+        <v>123</v>
+      </c>
+      <c r="E68" t="s">
+        <v>54</v>
+      </c>
+      <c r="F68" t="s">
         <v>249</v>
       </c>
-      <c r="D68" t="s">
-        <v>125</v>
-      </c>
-      <c r="E68" t="s">
-        <v>57</v>
-      </c>
-      <c r="F68" t="s">
-        <v>250</v>
-      </c>
       <c r="G68">
-        <v>2200000</v>
+        <v>2500000</v>
       </c>
       <c r="H68">
         <v>0</v>
       </c>
       <c r="I68">
-        <v>220000</v>
+        <v>250000</v>
       </c>
       <c r="J68">
-        <v>320000</v>
+        <v>370000</v>
       </c>
       <c r="K68">
         <v>0</v>
       </c>
       <c r="L68">
-        <v>440000</v>
+        <v>480000</v>
       </c>
       <c r="M68">
         <v>0</v>
@@ -4704,47 +4673,47 @@
         <v>0</v>
       </c>
       <c r="P68">
-        <v>1500000</v>
+        <v>1700000</v>
       </c>
       <c r="Q68">
-        <f t="shared" si="1"/>
-        <v>4680000</v>
+        <f t="shared" si="0"/>
+        <v>5300000</v>
       </c>
     </row>
     <row r="69" spans="1:47" customFormat="1">
       <c r="A69" s="4"/>
       <c r="B69" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C69" t="s">
+        <v>250</v>
+      </c>
+      <c r="D69" t="s">
+        <v>124</v>
+      </c>
+      <c r="E69" t="s">
+        <v>54</v>
+      </c>
+      <c r="F69" t="s">
         <v>251</v>
       </c>
-      <c r="D69" t="s">
-        <v>126</v>
-      </c>
-      <c r="E69" t="s">
-        <v>57</v>
-      </c>
-      <c r="F69" t="s">
-        <v>252</v>
-      </c>
       <c r="G69">
-        <v>2500000</v>
+        <v>1100000</v>
       </c>
       <c r="H69">
         <v>0</v>
       </c>
       <c r="I69">
-        <v>250000</v>
+        <v>110000</v>
       </c>
       <c r="J69">
-        <v>370000</v>
+        <v>165000</v>
       </c>
       <c r="K69">
         <v>0</v>
       </c>
       <c r="L69">
-        <v>480000</v>
+        <v>225000</v>
       </c>
       <c r="M69">
         <v>0</v>
@@ -4756,11 +4725,11 @@
         <v>0</v>
       </c>
       <c r="P69">
-        <v>1700000</v>
+        <v>780000</v>
       </c>
       <c r="Q69">
-        <f t="shared" si="1"/>
-        <v>5300000</v>
+        <f t="shared" si="0"/>
+        <v>2380000</v>
       </c>
     </row>
     <row r="70" spans="1:47" customFormat="1">
@@ -4769,34 +4738,34 @@
         <v>35</v>
       </c>
       <c r="C70" t="s">
+        <v>252</v>
+      </c>
+      <c r="D70" t="s">
+        <v>125</v>
+      </c>
+      <c r="E70" t="s">
+        <v>54</v>
+      </c>
+      <c r="F70" t="s">
         <v>253</v>
       </c>
-      <c r="D70" t="s">
-        <v>127</v>
-      </c>
-      <c r="E70" t="s">
-        <v>57</v>
-      </c>
-      <c r="F70" t="s">
-        <v>254</v>
-      </c>
       <c r="G70">
-        <v>1100000</v>
+        <v>780000</v>
       </c>
       <c r="H70">
         <v>0</v>
       </c>
       <c r="I70">
-        <v>110000</v>
+        <v>78000</v>
       </c>
       <c r="J70">
-        <v>165000</v>
+        <v>118000</v>
       </c>
       <c r="K70">
         <v>0</v>
       </c>
       <c r="L70">
-        <v>225000</v>
+        <v>154000</v>
       </c>
       <c r="M70">
         <v>0</v>
@@ -4808,151 +4777,112 @@
         <v>0</v>
       </c>
       <c r="P70">
-        <v>780000</v>
+        <v>550000</v>
       </c>
       <c r="Q70">
-        <f t="shared" si="1"/>
-        <v>2380000</v>
-      </c>
-    </row>
-    <row r="71" spans="1:47" customFormat="1">
-      <c r="A71" s="4"/>
-      <c r="B71" t="s">
-        <v>35</v>
-      </c>
-      <c r="C71" t="s">
-        <v>255</v>
-      </c>
-      <c r="D71" t="s">
-        <v>128</v>
-      </c>
-      <c r="E71" t="s">
-        <v>57</v>
-      </c>
-      <c r="F71" t="s">
-        <v>256</v>
-      </c>
-      <c r="G71">
-        <v>780000</v>
-      </c>
-      <c r="H71">
-        <v>0</v>
-      </c>
-      <c r="I71">
-        <v>78000</v>
-      </c>
-      <c r="J71">
-        <v>118000</v>
-      </c>
-      <c r="K71">
-        <v>0</v>
-      </c>
-      <c r="L71">
-        <v>154000</v>
-      </c>
-      <c r="M71">
-        <v>0</v>
-      </c>
-      <c r="N71">
-        <v>0</v>
-      </c>
-      <c r="O71">
-        <v>0</v>
-      </c>
-      <c r="P71">
-        <v>550000</v>
-      </c>
-      <c r="Q71">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1680000</v>
       </c>
     </row>
-    <row r="72" spans="1:47" ht="14.5" customHeight="1" outlineLevel="1">
-      <c r="B72" s="17"/>
+    <row r="71" spans="1:47" ht="14.5" customHeight="1" outlineLevel="1">
+      <c r="B71" s="12"/>
+      <c r="C71" s="12"/>
+      <c r="D71" s="12"/>
+      <c r="E71" s="12"/>
+      <c r="F71" s="12"/>
+      <c r="G71" s="12"/>
+      <c r="H71" s="12"/>
+      <c r="I71" s="12"/>
+      <c r="J71" s="12"/>
+      <c r="K71" s="12"/>
+      <c r="L71" s="12"/>
+      <c r="M71" s="12"/>
+      <c r="N71" s="12"/>
+      <c r="O71" s="12"/>
+      <c r="P71" s="12"/>
+      <c r="Q71" s="12"/>
+    </row>
+    <row r="72" spans="1:47" ht="14.5" customHeight="1">
+      <c r="B72" s="17" t="s">
+        <v>41</v>
+      </c>
       <c r="C72" s="17"/>
       <c r="D72" s="17"/>
-      <c r="E72" s="17"/>
-      <c r="F72" s="17"/>
-      <c r="G72" s="17"/>
-      <c r="H72" s="17"/>
-      <c r="I72" s="17"/>
-      <c r="J72" s="17"/>
-      <c r="K72" s="17"/>
-      <c r="L72" s="17"/>
-      <c r="M72" s="17"/>
-      <c r="N72" s="17"/>
-      <c r="O72" s="17"/>
-      <c r="P72" s="17"/>
-      <c r="Q72" s="17"/>
-    </row>
-    <row r="73" spans="1:47" ht="14.5" customHeight="1">
-      <c r="B73" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="C73" s="22"/>
-      <c r="D73" s="22"/>
-      <c r="E73" s="18"/>
-      <c r="F73" s="18"/>
-      <c r="G73" s="12">
-        <f t="shared" ref="G73:Q73" si="2">SUM(G8:G71)</f>
+      <c r="E72" s="13"/>
+      <c r="F72" s="13"/>
+      <c r="G72" s="10">
+        <f t="shared" ref="G72:P72" si="1">SUM(G7:G70)</f>
         <v>360620000</v>
       </c>
-      <c r="H73" s="12">
-        <f t="shared" si="2"/>
+      <c r="H72" s="10">
+        <f t="shared" si="1"/>
         <v>118954000</v>
       </c>
-      <c r="I73" s="12">
-        <f t="shared" si="2"/>
+      <c r="I72" s="10">
+        <f t="shared" si="1"/>
         <v>34784000</v>
       </c>
-      <c r="J73" s="12">
-        <f t="shared" si="2"/>
+      <c r="J72" s="10">
+        <f t="shared" si="1"/>
         <v>39663000</v>
       </c>
-      <c r="K73" s="12">
-        <f t="shared" si="2"/>
+      <c r="K72" s="10">
+        <f t="shared" si="1"/>
         <v>47997000</v>
       </c>
-      <c r="L73" s="12">
-        <f t="shared" si="2"/>
+      <c r="L72" s="10">
+        <f t="shared" si="1"/>
         <v>60632000</v>
       </c>
-      <c r="M73" s="12">
-        <f t="shared" si="2"/>
+      <c r="M72" s="10">
+        <f t="shared" si="1"/>
         <v>37100000</v>
       </c>
-      <c r="N73" s="12">
-        <f t="shared" si="2"/>
+      <c r="N72" s="10">
+        <f t="shared" si="1"/>
         <v>3500000</v>
       </c>
-      <c r="O73" s="12">
-        <f t="shared" si="2"/>
+      <c r="O72" s="10">
+        <f t="shared" si="1"/>
         <v>2950000</v>
       </c>
-      <c r="P73" s="12">
-        <f t="shared" si="2"/>
+      <c r="P72" s="10">
+        <f t="shared" si="1"/>
         <v>96380000</v>
       </c>
-      <c r="Q73" s="12">
-        <f>SUM(Q8:Q71)</f>
+      <c r="Q72" s="10">
+        <f>SUM(Q7:Q70)</f>
         <v>802580000</v>
       </c>
     </row>
+    <row r="73" spans="1:47">
+      <c r="G73" s="15"/>
+      <c r="H73" s="15"/>
+      <c r="I73" s="15"/>
+      <c r="J73" s="15"/>
+      <c r="K73" s="15"/>
+      <c r="L73" s="15"/>
+      <c r="M73" s="15"/>
+      <c r="N73" s="15"/>
+      <c r="O73" s="15"/>
+      <c r="P73" s="15"/>
+      <c r="Q73" s="15"/>
+    </row>
     <row r="74" spans="1:47">
-      <c r="G74" s="20"/>
-      <c r="H74" s="20"/>
-      <c r="I74" s="20"/>
-      <c r="J74" s="20"/>
-      <c r="K74" s="20"/>
-      <c r="L74" s="20"/>
-      <c r="M74" s="20"/>
-      <c r="N74" s="20"/>
-      <c r="O74" s="20"/>
-      <c r="P74" s="20"/>
-      <c r="Q74" s="20"/>
+      <c r="F74"/>
+      <c r="G74" s="4"/>
+      <c r="H74" s="4"/>
+      <c r="I74" s="4"/>
+      <c r="J74" s="4"/>
+      <c r="K74" s="4"/>
+      <c r="L74" s="4"/>
+      <c r="M74" s="4"/>
+      <c r="N74" s="4"/>
+      <c r="O74" s="4"/>
+      <c r="P74" s="4"/>
+      <c r="Q74" s="4"/>
     </row>
     <row r="75" spans="1:47">
-      <c r="F75"/>
       <c r="G75" s="4"/>
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
@@ -4966,22 +4896,54 @@
       <c r="Q75" s="4"/>
     </row>
     <row r="76" spans="1:47">
-      <c r="G76" s="4"/>
-      <c r="H76" s="4"/>
-      <c r="I76" s="4"/>
-      <c r="J76" s="4"/>
-      <c r="K76" s="4"/>
-      <c r="L76" s="4"/>
-      <c r="M76" s="4"/>
-      <c r="N76" s="4"/>
-      <c r="O76" s="4"/>
-      <c r="P76" s="4"/>
-      <c r="Q76" s="4"/>
-    </row>
-    <row r="77" spans="1:47">
-      <c r="A77" s="1"/>
+      <c r="A76" s="1"/>
+      <c r="C76" s="4"/>
+      <c r="N76" s="14"/>
+    </row>
+    <row r="77" spans="1:47" s="1" customFormat="1">
       <c r="C77" s="4"/>
-      <c r="N77" s="19"/>
+      <c r="F77" s="2"/>
+      <c r="G77" s="3"/>
+      <c r="H77" s="3"/>
+      <c r="I77" s="3"/>
+      <c r="J77" s="3"/>
+      <c r="K77" s="3"/>
+      <c r="L77" s="3"/>
+      <c r="M77" s="3"/>
+      <c r="N77" s="3"/>
+      <c r="O77" s="3"/>
+      <c r="P77" s="3"/>
+      <c r="Q77" s="3"/>
+      <c r="R77"/>
+      <c r="S77" s="4"/>
+      <c r="T77" s="4"/>
+      <c r="U77" s="4"/>
+      <c r="V77" s="4"/>
+      <c r="W77" s="4"/>
+      <c r="X77" s="4"/>
+      <c r="Y77" s="4"/>
+      <c r="Z77" s="4"/>
+      <c r="AA77" s="4"/>
+      <c r="AB77" s="4"/>
+      <c r="AC77" s="4"/>
+      <c r="AD77" s="4"/>
+      <c r="AE77" s="4"/>
+      <c r="AF77" s="4"/>
+      <c r="AG77" s="4"/>
+      <c r="AH77" s="4"/>
+      <c r="AI77" s="4"/>
+      <c r="AJ77" s="4"/>
+      <c r="AK77" s="4"/>
+      <c r="AL77" s="4"/>
+      <c r="AM77" s="4"/>
+      <c r="AN77" s="4"/>
+      <c r="AO77" s="4"/>
+      <c r="AP77" s="4"/>
+      <c r="AQ77" s="4"/>
+      <c r="AR77" s="4"/>
+      <c r="AS77" s="4"/>
+      <c r="AT77" s="4"/>
+      <c r="AU77" s="4"/>
     </row>
     <row r="78" spans="1:47" s="1" customFormat="1">
       <c r="C78" s="4"/>
@@ -5074,7 +5036,8 @@
       <c r="AU79" s="4"/>
     </row>
     <row r="80" spans="1:47" s="1" customFormat="1">
-      <c r="C80" s="4"/>
+      <c r="A80" s="4"/>
+      <c r="C80" s="5"/>
       <c r="F80" s="2"/>
       <c r="G80" s="3"/>
       <c r="H80" s="3"/>
@@ -5118,55 +5081,9 @@
       <c r="AT80" s="4"/>
       <c r="AU80" s="4"/>
     </row>
-    <row r="81" spans="1:47" s="1" customFormat="1">
-      <c r="A81" s="4"/>
-      <c r="C81" s="5"/>
-      <c r="F81" s="2"/>
-      <c r="G81" s="3"/>
-      <c r="H81" s="3"/>
-      <c r="I81" s="3"/>
-      <c r="J81" s="3"/>
-      <c r="K81" s="3"/>
-      <c r="L81" s="3"/>
-      <c r="M81" s="3"/>
-      <c r="N81" s="3"/>
-      <c r="O81" s="3"/>
-      <c r="P81" s="3"/>
-      <c r="Q81" s="3"/>
-      <c r="R81"/>
-      <c r="S81" s="4"/>
-      <c r="T81" s="4"/>
-      <c r="U81" s="4"/>
-      <c r="V81" s="4"/>
-      <c r="W81" s="4"/>
-      <c r="X81" s="4"/>
-      <c r="Y81" s="4"/>
-      <c r="Z81" s="4"/>
-      <c r="AA81" s="4"/>
-      <c r="AB81" s="4"/>
-      <c r="AC81" s="4"/>
-      <c r="AD81" s="4"/>
-      <c r="AE81" s="4"/>
-      <c r="AF81" s="4"/>
-      <c r="AG81" s="4"/>
-      <c r="AH81" s="4"/>
-      <c r="AI81" s="4"/>
-      <c r="AJ81" s="4"/>
-      <c r="AK81" s="4"/>
-      <c r="AL81" s="4"/>
-      <c r="AM81" s="4"/>
-      <c r="AN81" s="4"/>
-      <c r="AO81" s="4"/>
-      <c r="AP81" s="4"/>
-      <c r="AQ81" s="4"/>
-      <c r="AR81" s="4"/>
-      <c r="AS81" s="4"/>
-      <c r="AT81" s="4"/>
-      <c r="AU81" s="4"/>
-    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="B72:D72"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5174,26 +5091,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="72e9687c-dd16-42a4-b22f-37506a5a0d78" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca11ca2f-01e5-493b-bb15-47564d08beeb">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010056CB9BD5CCBAF1448722CAC9F0A67163" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d13d31ead20d27d69202087daf34c465">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ca11ca2f-01e5-493b-bb15-47564d08beeb" xmlns:ns3="72e9687c-dd16-42a4-b22f-37506a5a0d78" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ff65be263a3b8d3bd0dfe98e55cd9515" ns2:_="" ns3:_="">
     <xsd:import namespace="ca11ca2f-01e5-493b-bb15-47564d08beeb"/>
@@ -5454,28 +5351,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D5EA2B3-D5F1-4BCA-8B03-ACB94ED8953E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="29f32099-ee5a-49c0-9c71-92159c11c161"/>
-    <ds:schemaRef ds:uri="56377bc2-faa9-4f96-aa2c-273fb44c0c4d"/>
-    <ds:schemaRef ds:uri="72e9687c-dd16-42a4-b22f-37506a5a0d78"/>
-    <ds:schemaRef ds:uri="ca11ca2f-01e5-493b-bb15-47564d08beeb"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2544B30-2F4A-4C87-AE99-36BD3CF47B15}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="72e9687c-dd16-42a4-b22f-37506a5a0d78" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca11ca2f-01e5-493b-bb15-47564d08beeb">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD96D9B8-B63E-4365-8160-C5FD3331FA41}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5492,4 +5388,25 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2544B30-2F4A-4C87-AE99-36BD3CF47B15}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D5EA2B3-D5F1-4BCA-8B03-ACB94ED8953E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="29f32099-ee5a-49c0-9c71-92159c11c161"/>
+    <ds:schemaRef ds:uri="56377bc2-faa9-4f96-aa2c-273fb44c0c4d"/>
+    <ds:schemaRef ds:uri="72e9687c-dd16-42a4-b22f-37506a5a0d78"/>
+    <ds:schemaRef ds:uri="ca11ca2f-01e5-493b-bb15-47564d08beeb"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
iterating on insurance domain
</commit_message>
<xml_diff>
--- a/modules/Insurance/Files/Microsoft/2026/Microsoft.xlsx
+++ b/modules/Insurance/Files/Microsoft/2026/Microsoft.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://systemorph-my.sharepoint.com/personal/rbuergi_systemorph_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\MeshWeaver\modules\Insurance\Files\Microsoft\2026\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{37CFED4D-9876-4514-8893-9A71107E03D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6A33AB4-E925-45BD-839C-BAEDD97ED29B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9716AF-AF53-4237-9171-9C370C6AED8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6130" yWindow="3400" windowWidth="18720" windowHeight="12190" xr2:uid="{74B429DF-FE2F-4D9F-BEF1-C117811C90CF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16860" xr2:uid="{74B429DF-FE2F-4D9F-BEF1-C117811C90CF}"/>
   </bookViews>
   <sheets>
     <sheet name="2024 PDBI Values (Final)" sheetId="1" r:id="rId1"/>
@@ -827,10 +827,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="5">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$£-809]#,##0.00;\-#,##0.00;\-"/>
     <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="&quot;£&quot;#,##0"/>
+    <numFmt numFmtId="167" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -965,12 +967,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -993,9 +996,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1017,14 +1017,22 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="167" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{AA64FE36-CE35-4AE0-B15D-8DCA3D9DA79A}"/>
     <cellStyle name="Normal 2 2" xfId="2" xr:uid="{0E37C418-6CA4-4743-A22F-1C1520BA5223}"/>
@@ -1344,16 +1352,16 @@
   </sheetPr>
   <dimension ref="A1:AU80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P76" sqref="P76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="2.81640625" style="4" customWidth="1"/>
     <col min="2" max="2" width="29.7265625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="44.1796875" style="1" customWidth="1"/>
     <col min="5" max="5" width="22.54296875" style="1" customWidth="1"/>
     <col min="6" max="6" width="36.81640625" style="2" customWidth="1"/>
@@ -1369,17 +1377,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18.5">
-      <c r="B1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="10"/>
+      <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="9"/>
       <c r="Q1" s="4"/>
     </row>
     <row r="2" spans="1:18" ht="18.5">
       <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="16">
         <f>Q72</f>
         <v>802580000</v>
       </c>
@@ -1389,7 +1397,7 @@
       <c r="B3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="16">
         <v>5237100057</v>
       </c>
       <c r="Q3" s="4"/>
@@ -1398,7 +1406,7 @@
       <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="17">
         <f>SUM(C2:C3)</f>
         <v>6039680057</v>
       </c>
@@ -1406,52 +1414,52 @@
     </row>
     <row r="5" spans="1:18" customFormat="1"/>
     <row r="6" spans="1:18" s="6" customFormat="1" ht="18.5">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="J6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="L6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="M6" s="11" t="s">
+      <c r="M6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="N6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="O6" s="11" t="s">
+      <c r="O6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="P6" s="11" t="s">
+      <c r="P6" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="Q6" s="11" t="s">
+      <c r="Q6" s="10" t="s">
         <v>19</v>
       </c>
       <c r="R6"/>
@@ -1473,37 +1481,37 @@
       <c r="F7" t="s">
         <v>127</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="18">
         <v>125000000</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="18">
         <v>45000000</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="18">
         <v>12000000</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="18">
         <v>8500000</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="18">
         <v>15000000</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="18">
         <v>18000000</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="18">
         <v>22000000</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="18">
         <v>3500000</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="18">
         <v>1000000</v>
       </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
+      <c r="P7" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="18">
         <f>SUM(G7:P7)</f>
         <v>250000000</v>
       </c>
@@ -1525,37 +1533,37 @@
       <c r="F8" t="s">
         <v>129</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="18">
         <v>8500000</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="18">
         <v>3200000</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="18">
         <v>850000</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="18">
         <v>650000</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="18">
         <v>2500000</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="18">
         <v>1200000</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="18">
         <v>1800000</v>
       </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
+      <c r="N8" s="18">
+        <v>0</v>
+      </c>
+      <c r="O8" s="18">
         <v>300000</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="18">
         <v>2400000</v>
       </c>
-      <c r="Q8">
+      <c r="Q8" s="18">
         <f t="shared" ref="Q8:Q70" si="0">SUM(G8:P8)</f>
         <v>21400000</v>
       </c>
@@ -1577,37 +1585,37 @@
       <c r="F9" t="s">
         <v>131</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="18">
         <v>12000000</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="18">
         <v>4500000</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="18">
         <v>1100000</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="18">
         <v>950000</v>
       </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
+      <c r="K9" s="18">
+        <v>0</v>
+      </c>
+      <c r="L9" s="18">
         <v>2200000</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="18">
         <v>2500000</v>
       </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9">
+      <c r="N9" s="18">
+        <v>0</v>
+      </c>
+      <c r="O9" s="18">
         <v>750000</v>
       </c>
-      <c r="P9">
+      <c r="P9" s="18">
         <v>4800000</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" s="18">
         <f t="shared" si="0"/>
         <v>28800000</v>
       </c>
@@ -1629,37 +1637,37 @@
       <c r="F10" t="s">
         <v>133</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="18">
         <v>2100000</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="18">
         <v>800000</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="18">
         <v>220000</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="18">
         <v>450000</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="18">
         <v>1200000</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="18">
         <v>430000</v>
       </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
+      <c r="M10" s="18">
+        <v>0</v>
+      </c>
+      <c r="N10" s="18">
+        <v>0</v>
+      </c>
+      <c r="O10" s="18">
+        <v>0</v>
+      </c>
+      <c r="P10" s="18">
         <v>1200000</v>
       </c>
-      <c r="Q10">
+      <c r="Q10" s="18">
         <f t="shared" si="0"/>
         <v>6400000</v>
       </c>
@@ -1681,37 +1689,37 @@
       <c r="F11" t="s">
         <v>135</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="18">
         <v>2800000</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="18">
         <v>1050000</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="18">
         <v>280000</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="18">
         <v>320000</v>
       </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
+      <c r="K11" s="18">
+        <v>0</v>
+      </c>
+      <c r="L11" s="18">
         <v>650000</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="18">
         <v>500000</v>
       </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11">
+      <c r="N11" s="18">
+        <v>0</v>
+      </c>
+      <c r="O11" s="18">
+        <v>0</v>
+      </c>
+      <c r="P11" s="18">
         <v>1800000</v>
       </c>
-      <c r="Q11">
+      <c r="Q11" s="18">
         <f t="shared" si="0"/>
         <v>7400000</v>
       </c>
@@ -1733,37 +1741,37 @@
       <c r="F12" t="s">
         <v>137</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="18">
         <v>4200000</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="18">
         <v>1600000</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="18">
         <v>420000</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="18">
         <v>480000</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="18">
         <v>900000</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="18">
         <v>800000</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="18">
         <v>1000000</v>
       </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12">
+      <c r="N12" s="18">
+        <v>0</v>
+      </c>
+      <c r="O12" s="18">
+        <v>0</v>
+      </c>
+      <c r="P12" s="18">
         <v>2200000</v>
       </c>
-      <c r="Q12">
+      <c r="Q12" s="18">
         <f t="shared" si="0"/>
         <v>11600000</v>
       </c>
@@ -1785,37 +1793,37 @@
       <c r="F13" t="s">
         <v>139</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="18">
         <v>950000</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="18">
         <v>280000</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="18">
         <v>50000</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="18">
         <v>420000</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="18">
         <v>200000</v>
       </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-      <c r="P13">
-        <v>0</v>
-      </c>
-      <c r="Q13">
+      <c r="L13" s="18">
+        <v>0</v>
+      </c>
+      <c r="M13" s="18">
+        <v>0</v>
+      </c>
+      <c r="N13" s="18">
+        <v>0</v>
+      </c>
+      <c r="O13" s="18">
+        <v>0</v>
+      </c>
+      <c r="P13" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="18">
         <f t="shared" si="0"/>
         <v>1900000</v>
       </c>
@@ -1837,37 +1845,37 @@
       <c r="F14" t="s">
         <v>141</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="18">
         <v>2400000</v>
       </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
+      <c r="H14" s="18">
+        <v>0</v>
+      </c>
+      <c r="I14" s="18">
         <v>180000</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="18">
         <v>280000</v>
       </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14">
+      <c r="K14" s="18">
+        <v>0</v>
+      </c>
+      <c r="L14" s="18">
         <v>220000</v>
       </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
-      <c r="N14">
-        <v>0</v>
-      </c>
-      <c r="O14">
-        <v>0</v>
-      </c>
-      <c r="P14">
+      <c r="M14" s="18">
+        <v>0</v>
+      </c>
+      <c r="N14" s="18">
+        <v>0</v>
+      </c>
+      <c r="O14" s="18">
+        <v>0</v>
+      </c>
+      <c r="P14" s="18">
         <v>1500000</v>
       </c>
-      <c r="Q14">
+      <c r="Q14" s="18">
         <f t="shared" si="0"/>
         <v>4580000</v>
       </c>
@@ -1889,37 +1897,37 @@
       <c r="F15" t="s">
         <v>143</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="18">
         <v>1100000</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="18">
         <v>320000</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="18">
         <v>45000</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="18">
         <v>480000</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="18">
         <v>255000</v>
       </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15">
-        <v>0</v>
-      </c>
-      <c r="O15">
-        <v>0</v>
-      </c>
-      <c r="P15">
-        <v>0</v>
-      </c>
-      <c r="Q15">
+      <c r="L15" s="18">
+        <v>0</v>
+      </c>
+      <c r="M15" s="18">
+        <v>0</v>
+      </c>
+      <c r="N15" s="18">
+        <v>0</v>
+      </c>
+      <c r="O15" s="18">
+        <v>0</v>
+      </c>
+      <c r="P15" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="18">
         <f t="shared" si="0"/>
         <v>2200000</v>
       </c>
@@ -1941,37 +1949,37 @@
       <c r="F16" t="s">
         <v>145</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="18">
         <v>1600000</v>
       </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
+      <c r="H16" s="18">
+        <v>0</v>
+      </c>
+      <c r="I16" s="18">
         <v>150000</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="18">
         <v>220000</v>
       </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16">
+      <c r="K16" s="18">
+        <v>0</v>
+      </c>
+      <c r="L16" s="18">
         <v>180000</v>
       </c>
-      <c r="M16">
-        <v>0</v>
-      </c>
-      <c r="N16">
-        <v>0</v>
-      </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-      <c r="P16">
+      <c r="M16" s="18">
+        <v>0</v>
+      </c>
+      <c r="N16" s="18">
+        <v>0</v>
+      </c>
+      <c r="O16" s="18">
+        <v>0</v>
+      </c>
+      <c r="P16" s="18">
         <v>950000</v>
       </c>
-      <c r="Q16">
+      <c r="Q16" s="18">
         <f t="shared" si="0"/>
         <v>3100000</v>
       </c>
@@ -1993,37 +2001,37 @@
       <c r="F17" t="s">
         <v>147</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="18">
         <v>15000000</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="18">
         <v>5500000</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="18">
         <v>1400000</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="18">
         <v>1200000</v>
       </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
+      <c r="K17" s="18">
+        <v>0</v>
+      </c>
+      <c r="L17" s="18">
         <v>2800000</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="18">
         <v>3200000</v>
       </c>
-      <c r="N17">
-        <v>0</v>
-      </c>
-      <c r="O17">
+      <c r="N17" s="18">
+        <v>0</v>
+      </c>
+      <c r="O17" s="18">
         <v>900000</v>
       </c>
-      <c r="P17">
+      <c r="P17" s="18">
         <v>6500000</v>
       </c>
-      <c r="Q17">
+      <c r="Q17" s="18">
         <f t="shared" si="0"/>
         <v>36500000</v>
       </c>
@@ -2045,37 +2053,37 @@
       <c r="F18" t="s">
         <v>149</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="18">
         <v>7800000</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="18">
         <v>2900000</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="18">
         <v>780000</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="18">
         <v>920000</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="18">
         <v>1800000</v>
       </c>
-      <c r="L18">
+      <c r="L18" s="18">
         <v>1400000</v>
       </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="N18">
-        <v>0</v>
-      </c>
-      <c r="O18">
-        <v>0</v>
-      </c>
-      <c r="P18">
+      <c r="M18" s="18">
+        <v>0</v>
+      </c>
+      <c r="N18" s="18">
+        <v>0</v>
+      </c>
+      <c r="O18" s="18">
+        <v>0</v>
+      </c>
+      <c r="P18" s="18">
         <v>2100000</v>
       </c>
-      <c r="Q18">
+      <c r="Q18" s="18">
         <f t="shared" si="0"/>
         <v>17700000</v>
       </c>
@@ -2097,37 +2105,37 @@
       <c r="F19" t="s">
         <v>151</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="18">
         <v>6500000</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="18">
         <v>2400000</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="18">
         <v>650000</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="18">
         <v>750000</v>
       </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
+      <c r="K19" s="18">
+        <v>0</v>
+      </c>
+      <c r="L19" s="18">
         <v>1200000</v>
       </c>
-      <c r="M19">
+      <c r="M19" s="18">
         <v>1500000</v>
       </c>
-      <c r="N19">
-        <v>0</v>
-      </c>
-      <c r="O19">
-        <v>0</v>
-      </c>
-      <c r="P19">
+      <c r="N19" s="18">
+        <v>0</v>
+      </c>
+      <c r="O19" s="18">
+        <v>0</v>
+      </c>
+      <c r="P19" s="18">
         <v>3200000</v>
       </c>
-      <c r="Q19">
+      <c r="Q19" s="18">
         <f t="shared" si="0"/>
         <v>16200000</v>
       </c>
@@ -2149,37 +2157,37 @@
       <c r="F20" t="s">
         <v>153</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="18">
         <v>9200000</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="18">
         <v>3400000</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="18">
         <v>920000</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="18">
         <v>1050000</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="18">
         <v>2100000</v>
       </c>
-      <c r="L20">
+      <c r="L20" s="18">
         <v>1730000</v>
       </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
-      <c r="N20">
-        <v>0</v>
-      </c>
-      <c r="O20">
-        <v>0</v>
-      </c>
-      <c r="P20">
+      <c r="M20" s="18">
+        <v>0</v>
+      </c>
+      <c r="N20" s="18">
+        <v>0</v>
+      </c>
+      <c r="O20" s="18">
+        <v>0</v>
+      </c>
+      <c r="P20" s="18">
         <v>2800000</v>
       </c>
-      <c r="Q20">
+      <c r="Q20" s="18">
         <f t="shared" si="0"/>
         <v>21200000</v>
       </c>
@@ -2201,37 +2209,37 @@
       <c r="F21" t="s">
         <v>155</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="18">
         <v>3400000</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="18">
         <v>1250000</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="18">
         <v>340000</v>
       </c>
-      <c r="J21">
+      <c r="J21" s="18">
         <v>420000</v>
       </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21">
+      <c r="K21" s="18">
+        <v>0</v>
+      </c>
+      <c r="L21" s="18">
         <v>890000</v>
       </c>
-      <c r="M21">
+      <c r="M21" s="18">
         <v>500000</v>
       </c>
-      <c r="N21">
-        <v>0</v>
-      </c>
-      <c r="O21">
-        <v>0</v>
-      </c>
-      <c r="P21">
+      <c r="N21" s="18">
+        <v>0</v>
+      </c>
+      <c r="O21" s="18">
+        <v>0</v>
+      </c>
+      <c r="P21" s="18">
         <v>1900000</v>
       </c>
-      <c r="Q21">
+      <c r="Q21" s="18">
         <f t="shared" si="0"/>
         <v>8700000</v>
       </c>
@@ -2253,37 +2261,37 @@
       <c r="F22" t="s">
         <v>157</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="18">
         <v>2900000</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="18">
         <v>1100000</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="18">
         <v>290000</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="18">
         <v>350000</v>
       </c>
-      <c r="K22">
+      <c r="K22" s="18">
         <v>680000</v>
       </c>
-      <c r="L22">
+      <c r="L22" s="18">
         <v>480000</v>
       </c>
-      <c r="M22">
-        <v>0</v>
-      </c>
-      <c r="N22">
-        <v>0</v>
-      </c>
-      <c r="O22">
-        <v>0</v>
-      </c>
-      <c r="P22">
+      <c r="M22" s="18">
+        <v>0</v>
+      </c>
+      <c r="N22" s="18">
+        <v>0</v>
+      </c>
+      <c r="O22" s="18">
+        <v>0</v>
+      </c>
+      <c r="P22" s="18">
         <v>1600000</v>
       </c>
-      <c r="Q22">
+      <c r="Q22" s="18">
         <f t="shared" si="0"/>
         <v>7400000</v>
       </c>
@@ -2305,37 +2313,37 @@
       <c r="F23" t="s">
         <v>159</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="18">
         <v>2200000</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="18">
         <v>820000</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="18">
         <v>220000</v>
       </c>
-      <c r="J23">
+      <c r="J23" s="18">
         <v>280000</v>
       </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23">
+      <c r="K23" s="18">
+        <v>0</v>
+      </c>
+      <c r="L23" s="18">
         <v>580000</v>
       </c>
-      <c r="M23">
+      <c r="M23" s="18">
         <v>300000</v>
       </c>
-      <c r="N23">
-        <v>0</v>
-      </c>
-      <c r="O23">
-        <v>0</v>
-      </c>
-      <c r="P23">
+      <c r="N23" s="18">
+        <v>0</v>
+      </c>
+      <c r="O23" s="18">
+        <v>0</v>
+      </c>
+      <c r="P23" s="18">
         <v>1400000</v>
       </c>
-      <c r="Q23">
+      <c r="Q23" s="18">
         <f t="shared" si="0"/>
         <v>5800000</v>
       </c>
@@ -2357,37 +2365,37 @@
       <c r="F24" t="s">
         <v>161</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="18">
         <v>680000</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="18">
         <v>200000</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="18">
         <v>35000</v>
       </c>
-      <c r="J24">
+      <c r="J24" s="18">
         <v>310000</v>
       </c>
-      <c r="K24">
+      <c r="K24" s="18">
         <v>135000</v>
       </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
-      <c r="M24">
-        <v>0</v>
-      </c>
-      <c r="N24">
-        <v>0</v>
-      </c>
-      <c r="O24">
-        <v>0</v>
-      </c>
-      <c r="P24">
-        <v>0</v>
-      </c>
-      <c r="Q24">
+      <c r="L24" s="18">
+        <v>0</v>
+      </c>
+      <c r="M24" s="18">
+        <v>0</v>
+      </c>
+      <c r="N24" s="18">
+        <v>0</v>
+      </c>
+      <c r="O24" s="18">
+        <v>0</v>
+      </c>
+      <c r="P24" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="18">
         <f t="shared" si="0"/>
         <v>1360000</v>
       </c>
@@ -2409,37 +2417,37 @@
       <c r="F25" t="s">
         <v>163</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="18">
         <v>820000</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="18">
         <v>240000</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="18">
         <v>40000</v>
       </c>
-      <c r="J25">
+      <c r="J25" s="18">
         <v>370000</v>
       </c>
-      <c r="K25">
+      <c r="K25" s="18">
         <v>170000</v>
       </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
-      <c r="M25">
-        <v>0</v>
-      </c>
-      <c r="N25">
-        <v>0</v>
-      </c>
-      <c r="O25">
-        <v>0</v>
-      </c>
-      <c r="P25">
-        <v>0</v>
-      </c>
-      <c r="Q25">
+      <c r="L25" s="18">
+        <v>0</v>
+      </c>
+      <c r="M25" s="18">
+        <v>0</v>
+      </c>
+      <c r="N25" s="18">
+        <v>0</v>
+      </c>
+      <c r="O25" s="18">
+        <v>0</v>
+      </c>
+      <c r="P25" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="18">
         <f t="shared" si="0"/>
         <v>1640000</v>
       </c>
@@ -2461,37 +2469,37 @@
       <c r="F26" t="s">
         <v>165</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="18">
         <v>3100000</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="18">
         <v>1150000</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="18">
         <v>310000</v>
       </c>
-      <c r="J26">
+      <c r="J26" s="18">
         <v>380000</v>
       </c>
-      <c r="K26">
-        <v>0</v>
-      </c>
-      <c r="L26">
+      <c r="K26" s="18">
+        <v>0</v>
+      </c>
+      <c r="L26" s="18">
         <v>760000</v>
       </c>
-      <c r="M26">
+      <c r="M26" s="18">
         <v>500000</v>
       </c>
-      <c r="N26">
-        <v>0</v>
-      </c>
-      <c r="O26">
-        <v>0</v>
-      </c>
-      <c r="P26">
+      <c r="N26" s="18">
+        <v>0</v>
+      </c>
+      <c r="O26" s="18">
+        <v>0</v>
+      </c>
+      <c r="P26" s="18">
         <v>1800000</v>
       </c>
-      <c r="Q26">
+      <c r="Q26" s="18">
         <f t="shared" si="0"/>
         <v>8000000</v>
       </c>
@@ -2513,37 +2521,37 @@
       <c r="F27" t="s">
         <v>167</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="18">
         <v>18000000</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="18">
         <v>6500000</v>
       </c>
-      <c r="I27">
+      <c r="I27" s="18">
         <v>1800000</v>
       </c>
-      <c r="J27">
+      <c r="J27" s="18">
         <v>2100000</v>
       </c>
-      <c r="K27">
+      <c r="K27" s="18">
         <v>4200000</v>
       </c>
-      <c r="L27">
+      <c r="L27" s="18">
         <v>3400000</v>
       </c>
-      <c r="M27">
-        <v>0</v>
-      </c>
-      <c r="N27">
-        <v>0</v>
-      </c>
-      <c r="O27">
-        <v>0</v>
-      </c>
-      <c r="P27">
+      <c r="M27" s="18">
+        <v>0</v>
+      </c>
+      <c r="N27" s="18">
+        <v>0</v>
+      </c>
+      <c r="O27" s="18">
+        <v>0</v>
+      </c>
+      <c r="P27" s="18">
         <v>4500000</v>
       </c>
-      <c r="Q27">
+      <c r="Q27" s="18">
         <f t="shared" si="0"/>
         <v>40500000</v>
       </c>
@@ -2565,37 +2573,37 @@
       <c r="F28" t="s">
         <v>169</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="18">
         <v>12500000</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="18">
         <v>4600000</v>
       </c>
-      <c r="I28">
+      <c r="I28" s="18">
         <v>1250000</v>
       </c>
-      <c r="J28">
+      <c r="J28" s="18">
         <v>1480000</v>
       </c>
-      <c r="K28">
+      <c r="K28" s="18">
         <v>2800000</v>
       </c>
-      <c r="L28">
+      <c r="L28" s="18">
         <v>2370000</v>
       </c>
-      <c r="M28">
-        <v>0</v>
-      </c>
-      <c r="N28">
-        <v>0</v>
-      </c>
-      <c r="O28">
-        <v>0</v>
-      </c>
-      <c r="P28">
+      <c r="M28" s="18">
+        <v>0</v>
+      </c>
+      <c r="N28" s="18">
+        <v>0</v>
+      </c>
+      <c r="O28" s="18">
+        <v>0</v>
+      </c>
+      <c r="P28" s="18">
         <v>3200000</v>
       </c>
-      <c r="Q28">
+      <c r="Q28" s="18">
         <f t="shared" si="0"/>
         <v>28200000</v>
       </c>
@@ -2617,37 +2625,37 @@
       <c r="F29" t="s">
         <v>171</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="18">
         <v>7200000</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="18">
         <v>2650000</v>
       </c>
-      <c r="I29">
+      <c r="I29" s="18">
         <v>720000</v>
       </c>
-      <c r="J29">
+      <c r="J29" s="18">
         <v>850000</v>
       </c>
-      <c r="K29">
+      <c r="K29" s="18">
         <v>1800000</v>
       </c>
-      <c r="L29">
+      <c r="L29" s="18">
         <v>1180000</v>
       </c>
-      <c r="M29">
-        <v>0</v>
-      </c>
-      <c r="N29">
-        <v>0</v>
-      </c>
-      <c r="O29">
-        <v>0</v>
-      </c>
-      <c r="P29">
+      <c r="M29" s="18">
+        <v>0</v>
+      </c>
+      <c r="N29" s="18">
+        <v>0</v>
+      </c>
+      <c r="O29" s="18">
+        <v>0</v>
+      </c>
+      <c r="P29" s="18">
         <v>2100000</v>
       </c>
-      <c r="Q29">
+      <c r="Q29" s="18">
         <f t="shared" si="0"/>
         <v>16500000</v>
       </c>
@@ -2669,37 +2677,37 @@
       <c r="F30" t="s">
         <v>173</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="18">
         <v>9800000</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="18">
         <v>3600000</v>
       </c>
-      <c r="I30">
+      <c r="I30" s="18">
         <v>980000</v>
       </c>
-      <c r="J30">
+      <c r="J30" s="18">
         <v>1150000</v>
       </c>
-      <c r="K30">
-        <v>0</v>
-      </c>
-      <c r="L30">
+      <c r="K30" s="18">
+        <v>0</v>
+      </c>
+      <c r="L30" s="18">
         <v>2270000</v>
       </c>
-      <c r="M30">
+      <c r="M30" s="18">
         <v>1800000</v>
       </c>
-      <c r="N30">
-        <v>0</v>
-      </c>
-      <c r="O30">
-        <v>0</v>
-      </c>
-      <c r="P30">
+      <c r="N30" s="18">
+        <v>0</v>
+      </c>
+      <c r="O30" s="18">
+        <v>0</v>
+      </c>
+      <c r="P30" s="18">
         <v>5200000</v>
       </c>
-      <c r="Q30">
+      <c r="Q30" s="18">
         <f t="shared" si="0"/>
         <v>24800000</v>
       </c>
@@ -2721,37 +2729,37 @@
       <c r="F31" t="s">
         <v>175</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="18">
         <v>2600000</v>
       </c>
-      <c r="H31">
-        <v>0</v>
-      </c>
-      <c r="I31">
+      <c r="H31" s="18">
+        <v>0</v>
+      </c>
+      <c r="I31" s="18">
         <v>280000</v>
       </c>
-      <c r="J31">
+      <c r="J31" s="18">
         <v>380000</v>
       </c>
-      <c r="K31">
-        <v>0</v>
-      </c>
-      <c r="L31">
+      <c r="K31" s="18">
+        <v>0</v>
+      </c>
+      <c r="L31" s="18">
         <v>440000</v>
       </c>
-      <c r="M31">
-        <v>0</v>
-      </c>
-      <c r="N31">
-        <v>0</v>
-      </c>
-      <c r="O31">
-        <v>0</v>
-      </c>
-      <c r="P31">
+      <c r="M31" s="18">
+        <v>0</v>
+      </c>
+      <c r="N31" s="18">
+        <v>0</v>
+      </c>
+      <c r="O31" s="18">
+        <v>0</v>
+      </c>
+      <c r="P31" s="18">
         <v>1800000</v>
       </c>
-      <c r="Q31">
+      <c r="Q31" s="18">
         <f t="shared" si="0"/>
         <v>5500000</v>
       </c>
@@ -2773,37 +2781,37 @@
       <c r="F32" t="s">
         <v>177</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="18">
         <v>5400000</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="18">
         <v>2000000</v>
       </c>
-      <c r="I32">
+      <c r="I32" s="18">
         <v>540000</v>
       </c>
-      <c r="J32">
+      <c r="J32" s="18">
         <v>650000</v>
       </c>
-      <c r="K32">
-        <v>0</v>
-      </c>
-      <c r="L32">
+      <c r="K32" s="18">
+        <v>0</v>
+      </c>
+      <c r="L32" s="18">
         <v>1210000</v>
       </c>
-      <c r="M32">
+      <c r="M32" s="18">
         <v>1000000</v>
       </c>
-      <c r="N32">
-        <v>0</v>
-      </c>
-      <c r="O32">
-        <v>0</v>
-      </c>
-      <c r="P32">
+      <c r="N32" s="18">
+        <v>0</v>
+      </c>
+      <c r="O32" s="18">
+        <v>0</v>
+      </c>
+      <c r="P32" s="18">
         <v>2900000</v>
       </c>
-      <c r="Q32">
+      <c r="Q32" s="18">
         <f t="shared" si="0"/>
         <v>13700000</v>
       </c>
@@ -2825,37 +2833,37 @@
       <c r="F33" t="s">
         <v>179</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="18">
         <v>720000</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="18">
         <v>210000</v>
       </c>
-      <c r="I33">
+      <c r="I33" s="18">
         <v>38000</v>
       </c>
-      <c r="J33">
+      <c r="J33" s="18">
         <v>330000</v>
       </c>
-      <c r="K33">
+      <c r="K33" s="18">
         <v>142000</v>
       </c>
-      <c r="L33">
-        <v>0</v>
-      </c>
-      <c r="M33">
-        <v>0</v>
-      </c>
-      <c r="N33">
-        <v>0</v>
-      </c>
-      <c r="O33">
-        <v>0</v>
-      </c>
-      <c r="P33">
-        <v>0</v>
-      </c>
-      <c r="Q33">
+      <c r="L33" s="18">
+        <v>0</v>
+      </c>
+      <c r="M33" s="18">
+        <v>0</v>
+      </c>
+      <c r="N33" s="18">
+        <v>0</v>
+      </c>
+      <c r="O33" s="18">
+        <v>0</v>
+      </c>
+      <c r="P33" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="18">
         <f t="shared" si="0"/>
         <v>1440000</v>
       </c>
@@ -2877,37 +2885,37 @@
       <c r="F34" t="s">
         <v>181</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="18">
         <v>16000000</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="18">
         <v>5800000</v>
       </c>
-      <c r="I34">
+      <c r="I34" s="18">
         <v>1600000</v>
       </c>
-      <c r="J34">
+      <c r="J34" s="18">
         <v>1900000</v>
       </c>
-      <c r="K34">
+      <c r="K34" s="18">
         <v>3500000</v>
       </c>
-      <c r="L34">
+      <c r="L34" s="18">
         <v>3200000</v>
       </c>
-      <c r="M34">
-        <v>0</v>
-      </c>
-      <c r="N34">
-        <v>0</v>
-      </c>
-      <c r="O34">
-        <v>0</v>
-      </c>
-      <c r="P34">
+      <c r="M34" s="18">
+        <v>0</v>
+      </c>
+      <c r="N34" s="18">
+        <v>0</v>
+      </c>
+      <c r="O34" s="18">
+        <v>0</v>
+      </c>
+      <c r="P34" s="18">
         <v>3800000</v>
       </c>
-      <c r="Q34">
+      <c r="Q34" s="18">
         <f t="shared" si="0"/>
         <v>35800000</v>
       </c>
@@ -2929,37 +2937,37 @@
       <c r="F35" t="s">
         <v>183</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="18">
         <v>11500000</v>
       </c>
-      <c r="H35">
+      <c r="H35" s="18">
         <v>4200000</v>
       </c>
-      <c r="I35">
+      <c r="I35" s="18">
         <v>1150000</v>
       </c>
-      <c r="J35">
+      <c r="J35" s="18">
         <v>1380000</v>
       </c>
-      <c r="K35">
+      <c r="K35" s="18">
         <v>2600000</v>
       </c>
-      <c r="L35">
+      <c r="L35" s="18">
         <v>2170000</v>
       </c>
-      <c r="M35">
-        <v>0</v>
-      </c>
-      <c r="N35">
-        <v>0</v>
-      </c>
-      <c r="O35">
-        <v>0</v>
-      </c>
-      <c r="P35">
+      <c r="M35" s="18">
+        <v>0</v>
+      </c>
+      <c r="N35" s="18">
+        <v>0</v>
+      </c>
+      <c r="O35" s="18">
+        <v>0</v>
+      </c>
+      <c r="P35" s="18">
         <v>2800000</v>
       </c>
-      <c r="Q35">
+      <c r="Q35" s="18">
         <f t="shared" si="0"/>
         <v>25800000</v>
       </c>
@@ -2981,37 +2989,37 @@
       <c r="F36" t="s">
         <v>185</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="18">
         <v>3200000</v>
       </c>
-      <c r="H36">
-        <v>0</v>
-      </c>
-      <c r="I36">
+      <c r="H36" s="18">
+        <v>0</v>
+      </c>
+      <c r="I36" s="18">
         <v>320000</v>
       </c>
-      <c r="J36">
+      <c r="J36" s="18">
         <v>460000</v>
       </c>
-      <c r="K36">
-        <v>0</v>
-      </c>
-      <c r="L36">
+      <c r="K36" s="18">
+        <v>0</v>
+      </c>
+      <c r="L36" s="18">
         <v>620000</v>
       </c>
-      <c r="M36">
-        <v>0</v>
-      </c>
-      <c r="N36">
-        <v>0</v>
-      </c>
-      <c r="O36">
-        <v>0</v>
-      </c>
-      <c r="P36">
+      <c r="M36" s="18">
+        <v>0</v>
+      </c>
+      <c r="N36" s="18">
+        <v>0</v>
+      </c>
+      <c r="O36" s="18">
+        <v>0</v>
+      </c>
+      <c r="P36" s="18">
         <v>2100000</v>
       </c>
-      <c r="Q36">
+      <c r="Q36" s="18">
         <f t="shared" si="0"/>
         <v>6700000</v>
       </c>
@@ -3033,37 +3041,37 @@
       <c r="F37" t="s">
         <v>187</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="18">
         <v>6200000</v>
       </c>
-      <c r="H37">
+      <c r="H37" s="18">
         <v>2300000</v>
       </c>
-      <c r="I37">
+      <c r="I37" s="18">
         <v>620000</v>
       </c>
-      <c r="J37">
+      <c r="J37" s="18">
         <v>740000</v>
       </c>
-      <c r="K37">
+      <c r="K37" s="18">
         <v>1400000</v>
       </c>
-      <c r="L37">
+      <c r="L37" s="18">
         <v>1140000</v>
       </c>
-      <c r="M37">
-        <v>0</v>
-      </c>
-      <c r="N37">
-        <v>0</v>
-      </c>
-      <c r="O37">
-        <v>0</v>
-      </c>
-      <c r="P37">
+      <c r="M37" s="18">
+        <v>0</v>
+      </c>
+      <c r="N37" s="18">
+        <v>0</v>
+      </c>
+      <c r="O37" s="18">
+        <v>0</v>
+      </c>
+      <c r="P37" s="18">
         <v>2500000</v>
       </c>
-      <c r="Q37">
+      <c r="Q37" s="18">
         <f t="shared" si="0"/>
         <v>14900000</v>
       </c>
@@ -3085,37 +3093,37 @@
       <c r="F38" t="s">
         <v>189</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="18">
         <v>4800000</v>
       </c>
-      <c r="H38">
+      <c r="H38" s="18">
         <v>1800000</v>
       </c>
-      <c r="I38">
+      <c r="I38" s="18">
         <v>480000</v>
       </c>
-      <c r="J38">
+      <c r="J38" s="18">
         <v>580000</v>
       </c>
-      <c r="K38">
+      <c r="K38" s="18">
         <v>1100000</v>
       </c>
-      <c r="L38">
+      <c r="L38" s="18">
         <v>840000</v>
       </c>
-      <c r="M38">
-        <v>0</v>
-      </c>
-      <c r="N38">
-        <v>0</v>
-      </c>
-      <c r="O38">
-        <v>0</v>
-      </c>
-      <c r="P38">
+      <c r="M38" s="18">
+        <v>0</v>
+      </c>
+      <c r="N38" s="18">
+        <v>0</v>
+      </c>
+      <c r="O38" s="18">
+        <v>0</v>
+      </c>
+      <c r="P38" s="18">
         <v>2200000</v>
       </c>
-      <c r="Q38">
+      <c r="Q38" s="18">
         <f t="shared" si="0"/>
         <v>11800000</v>
       </c>
@@ -3137,37 +3145,37 @@
       <c r="F39" t="s">
         <v>191</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="18">
         <v>2900000</v>
       </c>
-      <c r="H39">
+      <c r="H39" s="18">
         <v>1100000</v>
       </c>
-      <c r="I39">
+      <c r="I39" s="18">
         <v>290000</v>
       </c>
-      <c r="J39">
+      <c r="J39" s="18">
         <v>350000</v>
       </c>
-      <c r="K39">
+      <c r="K39" s="18">
         <v>680000</v>
       </c>
-      <c r="L39">
+      <c r="L39" s="18">
         <v>480000</v>
       </c>
-      <c r="M39">
-        <v>0</v>
-      </c>
-      <c r="N39">
-        <v>0</v>
-      </c>
-      <c r="O39">
-        <v>0</v>
-      </c>
-      <c r="P39">
+      <c r="M39" s="18">
+        <v>0</v>
+      </c>
+      <c r="N39" s="18">
+        <v>0</v>
+      </c>
+      <c r="O39" s="18">
+        <v>0</v>
+      </c>
+      <c r="P39" s="18">
         <v>1600000</v>
       </c>
-      <c r="Q39">
+      <c r="Q39" s="18">
         <f t="shared" si="0"/>
         <v>7400000</v>
       </c>
@@ -3189,37 +3197,37 @@
       <c r="F40" t="s">
         <v>193</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="18">
         <v>2400000</v>
       </c>
-      <c r="H40">
-        <v>0</v>
-      </c>
-      <c r="I40">
+      <c r="H40" s="18">
+        <v>0</v>
+      </c>
+      <c r="I40" s="18">
         <v>240000</v>
       </c>
-      <c r="J40">
+      <c r="J40" s="18">
         <v>340000</v>
       </c>
-      <c r="K40">
-        <v>0</v>
-      </c>
-      <c r="L40">
+      <c r="K40" s="18">
+        <v>0</v>
+      </c>
+      <c r="L40" s="18">
         <v>520000</v>
       </c>
-      <c r="M40">
-        <v>0</v>
-      </c>
-      <c r="N40">
-        <v>0</v>
-      </c>
-      <c r="O40">
-        <v>0</v>
-      </c>
-      <c r="P40">
+      <c r="M40" s="18">
+        <v>0</v>
+      </c>
+      <c r="N40" s="18">
+        <v>0</v>
+      </c>
+      <c r="O40" s="18">
+        <v>0</v>
+      </c>
+      <c r="P40" s="18">
         <v>1900000</v>
       </c>
-      <c r="Q40">
+      <c r="Q40" s="18">
         <f t="shared" si="0"/>
         <v>5400000</v>
       </c>
@@ -3241,37 +3249,37 @@
       <c r="F41" t="s">
         <v>195</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="18">
         <v>1400000</v>
       </c>
-      <c r="H41">
-        <v>0</v>
-      </c>
-      <c r="I41">
+      <c r="H41" s="18">
+        <v>0</v>
+      </c>
+      <c r="I41" s="18">
         <v>140000</v>
       </c>
-      <c r="J41">
+      <c r="J41" s="18">
         <v>200000</v>
       </c>
-      <c r="K41">
-        <v>0</v>
-      </c>
-      <c r="L41">
+      <c r="K41" s="18">
+        <v>0</v>
+      </c>
+      <c r="L41" s="18">
         <v>260000</v>
       </c>
-      <c r="M41">
-        <v>0</v>
-      </c>
-      <c r="N41">
-        <v>0</v>
-      </c>
-      <c r="O41">
-        <v>0</v>
-      </c>
-      <c r="P41">
+      <c r="M41" s="18">
+        <v>0</v>
+      </c>
+      <c r="N41" s="18">
+        <v>0</v>
+      </c>
+      <c r="O41" s="18">
+        <v>0</v>
+      </c>
+      <c r="P41" s="18">
         <v>980000</v>
       </c>
-      <c r="Q41">
+      <c r="Q41" s="18">
         <f t="shared" si="0"/>
         <v>2980000</v>
       </c>
@@ -3293,37 +3301,37 @@
       <c r="F42" t="s">
         <v>197</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="18">
         <v>1600000</v>
       </c>
-      <c r="H42">
-        <v>0</v>
-      </c>
-      <c r="I42">
+      <c r="H42" s="18">
+        <v>0</v>
+      </c>
+      <c r="I42" s="18">
         <v>160000</v>
       </c>
-      <c r="J42">
+      <c r="J42" s="18">
         <v>230000</v>
       </c>
-      <c r="K42">
-        <v>0</v>
-      </c>
-      <c r="L42">
+      <c r="K42" s="18">
+        <v>0</v>
+      </c>
+      <c r="L42" s="18">
         <v>310000</v>
       </c>
-      <c r="M42">
-        <v>0</v>
-      </c>
-      <c r="N42">
-        <v>0</v>
-      </c>
-      <c r="O42">
-        <v>0</v>
-      </c>
-      <c r="P42">
+      <c r="M42" s="18">
+        <v>0</v>
+      </c>
+      <c r="N42" s="18">
+        <v>0</v>
+      </c>
+      <c r="O42" s="18">
+        <v>0</v>
+      </c>
+      <c r="P42" s="18">
         <v>1100000</v>
       </c>
-      <c r="Q42">
+      <c r="Q42" s="18">
         <f t="shared" si="0"/>
         <v>3400000</v>
       </c>
@@ -3345,37 +3353,37 @@
       <c r="F43" t="s">
         <v>199</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="18">
         <v>1200000</v>
       </c>
-      <c r="H43">
-        <v>0</v>
-      </c>
-      <c r="I43">
+      <c r="H43" s="18">
+        <v>0</v>
+      </c>
+      <c r="I43" s="18">
         <v>120000</v>
       </c>
-      <c r="J43">
+      <c r="J43" s="18">
         <v>180000</v>
       </c>
-      <c r="K43">
-        <v>0</v>
-      </c>
-      <c r="L43">
+      <c r="K43" s="18">
+        <v>0</v>
+      </c>
+      <c r="L43" s="18">
         <v>220000</v>
       </c>
-      <c r="M43">
-        <v>0</v>
-      </c>
-      <c r="N43">
-        <v>0</v>
-      </c>
-      <c r="O43">
-        <v>0</v>
-      </c>
-      <c r="P43">
+      <c r="M43" s="18">
+        <v>0</v>
+      </c>
+      <c r="N43" s="18">
+        <v>0</v>
+      </c>
+      <c r="O43" s="18">
+        <v>0</v>
+      </c>
+      <c r="P43" s="18">
         <v>850000</v>
       </c>
-      <c r="Q43">
+      <c r="Q43" s="18">
         <f t="shared" si="0"/>
         <v>2570000</v>
       </c>
@@ -3397,37 +3405,37 @@
       <c r="F44" t="s">
         <v>201</v>
       </c>
-      <c r="G44">
+      <c r="G44" s="18">
         <v>1050000</v>
       </c>
-      <c r="H44">
-        <v>0</v>
-      </c>
-      <c r="I44">
+      <c r="H44" s="18">
+        <v>0</v>
+      </c>
+      <c r="I44" s="18">
         <v>105000</v>
       </c>
-      <c r="J44">
+      <c r="J44" s="18">
         <v>160000</v>
       </c>
-      <c r="K44">
-        <v>0</v>
-      </c>
-      <c r="L44">
+      <c r="K44" s="18">
+        <v>0</v>
+      </c>
+      <c r="L44" s="18">
         <v>185000</v>
       </c>
-      <c r="M44">
-        <v>0</v>
-      </c>
-      <c r="N44">
-        <v>0</v>
-      </c>
-      <c r="O44">
-        <v>0</v>
-      </c>
-      <c r="P44">
+      <c r="M44" s="18">
+        <v>0</v>
+      </c>
+      <c r="N44" s="18">
+        <v>0</v>
+      </c>
+      <c r="O44" s="18">
+        <v>0</v>
+      </c>
+      <c r="P44" s="18">
         <v>750000</v>
       </c>
-      <c r="Q44">
+      <c r="Q44" s="18">
         <f t="shared" si="0"/>
         <v>2250000</v>
       </c>
@@ -3449,37 +3457,37 @@
       <c r="F45" t="s">
         <v>203</v>
       </c>
-      <c r="G45">
+      <c r="G45" s="18">
         <v>890000</v>
       </c>
-      <c r="H45">
-        <v>0</v>
-      </c>
-      <c r="I45">
+      <c r="H45" s="18">
+        <v>0</v>
+      </c>
+      <c r="I45" s="18">
         <v>89000</v>
       </c>
-      <c r="J45">
+      <c r="J45" s="18">
         <v>135000</v>
       </c>
-      <c r="K45">
-        <v>0</v>
-      </c>
-      <c r="L45">
+      <c r="K45" s="18">
+        <v>0</v>
+      </c>
+      <c r="L45" s="18">
         <v>166000</v>
       </c>
-      <c r="M45">
-        <v>0</v>
-      </c>
-      <c r="N45">
-        <v>0</v>
-      </c>
-      <c r="O45">
-        <v>0</v>
-      </c>
-      <c r="P45">
+      <c r="M45" s="18">
+        <v>0</v>
+      </c>
+      <c r="N45" s="18">
+        <v>0</v>
+      </c>
+      <c r="O45" s="18">
+        <v>0</v>
+      </c>
+      <c r="P45" s="18">
         <v>650000</v>
       </c>
-      <c r="Q45">
+      <c r="Q45" s="18">
         <f t="shared" si="0"/>
         <v>1930000</v>
       </c>
@@ -3501,37 +3509,37 @@
       <c r="F46" t="s">
         <v>205</v>
       </c>
-      <c r="G46">
+      <c r="G46" s="18">
         <v>2800000</v>
       </c>
-      <c r="H46">
+      <c r="H46" s="18">
         <v>1050000</v>
       </c>
-      <c r="I46">
+      <c r="I46" s="18">
         <v>280000</v>
       </c>
-      <c r="J46">
+      <c r="J46" s="18">
         <v>340000</v>
       </c>
-      <c r="K46">
-        <v>0</v>
-      </c>
-      <c r="L46">
+      <c r="K46" s="18">
+        <v>0</v>
+      </c>
+      <c r="L46" s="18">
         <v>630000</v>
       </c>
-      <c r="M46">
+      <c r="M46" s="18">
         <v>500000</v>
       </c>
-      <c r="N46">
-        <v>0</v>
-      </c>
-      <c r="O46">
-        <v>0</v>
-      </c>
-      <c r="P46">
+      <c r="N46" s="18">
+        <v>0</v>
+      </c>
+      <c r="O46" s="18">
+        <v>0</v>
+      </c>
+      <c r="P46" s="18">
         <v>1800000</v>
       </c>
-      <c r="Q46">
+      <c r="Q46" s="18">
         <f t="shared" si="0"/>
         <v>7400000</v>
       </c>
@@ -3553,37 +3561,37 @@
       <c r="F47" t="s">
         <v>207</v>
       </c>
-      <c r="G47">
+      <c r="G47" s="18">
         <v>2100000</v>
       </c>
-      <c r="H47">
+      <c r="H47" s="18">
         <v>780000</v>
       </c>
-      <c r="I47">
+      <c r="I47" s="18">
         <v>210000</v>
       </c>
-      <c r="J47">
+      <c r="J47" s="18">
         <v>250000</v>
       </c>
-      <c r="K47">
+      <c r="K47" s="18">
         <v>520000</v>
       </c>
-      <c r="L47">
+      <c r="L47" s="18">
         <v>340000</v>
       </c>
-      <c r="M47">
-        <v>0</v>
-      </c>
-      <c r="N47">
-        <v>0</v>
-      </c>
-      <c r="O47">
-        <v>0</v>
-      </c>
-      <c r="P47">
+      <c r="M47" s="18">
+        <v>0</v>
+      </c>
+      <c r="N47" s="18">
+        <v>0</v>
+      </c>
+      <c r="O47" s="18">
+        <v>0</v>
+      </c>
+      <c r="P47" s="18">
         <v>1200000</v>
       </c>
-      <c r="Q47">
+      <c r="Q47" s="18">
         <f t="shared" si="0"/>
         <v>5400000</v>
       </c>
@@ -3605,37 +3613,37 @@
       <c r="F48" t="s">
         <v>209</v>
       </c>
-      <c r="G48">
+      <c r="G48" s="18">
         <v>4500000</v>
       </c>
-      <c r="H48">
+      <c r="H48" s="18">
         <v>1650000</v>
       </c>
-      <c r="I48">
+      <c r="I48" s="18">
         <v>450000</v>
       </c>
-      <c r="J48">
+      <c r="J48" s="18">
         <v>540000</v>
       </c>
-      <c r="K48">
+      <c r="K48" s="18">
         <v>1050000</v>
       </c>
-      <c r="L48">
+      <c r="L48" s="18">
         <v>810000</v>
       </c>
-      <c r="M48">
-        <v>0</v>
-      </c>
-      <c r="N48">
-        <v>0</v>
-      </c>
-      <c r="O48">
-        <v>0</v>
-      </c>
-      <c r="P48">
+      <c r="M48" s="18">
+        <v>0</v>
+      </c>
+      <c r="N48" s="18">
+        <v>0</v>
+      </c>
+      <c r="O48" s="18">
+        <v>0</v>
+      </c>
+      <c r="P48" s="18">
         <v>1900000</v>
       </c>
-      <c r="Q48">
+      <c r="Q48" s="18">
         <f t="shared" si="0"/>
         <v>10900000</v>
       </c>
@@ -3657,37 +3665,37 @@
       <c r="F49" t="s">
         <v>211</v>
       </c>
-      <c r="G49">
+      <c r="G49" s="18">
         <v>1150000</v>
       </c>
-      <c r="H49">
-        <v>0</v>
-      </c>
-      <c r="I49">
+      <c r="H49" s="18">
+        <v>0</v>
+      </c>
+      <c r="I49" s="18">
         <v>115000</v>
       </c>
-      <c r="J49">
+      <c r="J49" s="18">
         <v>175000</v>
       </c>
-      <c r="K49">
-        <v>0</v>
-      </c>
-      <c r="L49">
+      <c r="K49" s="18">
+        <v>0</v>
+      </c>
+      <c r="L49" s="18">
         <v>210000</v>
       </c>
-      <c r="M49">
-        <v>0</v>
-      </c>
-      <c r="N49">
-        <v>0</v>
-      </c>
-      <c r="O49">
-        <v>0</v>
-      </c>
-      <c r="P49">
+      <c r="M49" s="18">
+        <v>0</v>
+      </c>
+      <c r="N49" s="18">
+        <v>0</v>
+      </c>
+      <c r="O49" s="18">
+        <v>0</v>
+      </c>
+      <c r="P49" s="18">
         <v>800000</v>
       </c>
-      <c r="Q49">
+      <c r="Q49" s="18">
         <f t="shared" si="0"/>
         <v>2450000</v>
       </c>
@@ -3709,37 +3717,37 @@
       <c r="F50" t="s">
         <v>213</v>
       </c>
-      <c r="G50">
+      <c r="G50" s="18">
         <v>580000</v>
       </c>
-      <c r="H50">
+      <c r="H50" s="18">
         <v>170000</v>
       </c>
-      <c r="I50">
+      <c r="I50" s="18">
         <v>30000</v>
       </c>
-      <c r="J50">
+      <c r="J50" s="18">
         <v>265000</v>
       </c>
-      <c r="K50">
+      <c r="K50" s="18">
         <v>115000</v>
       </c>
-      <c r="L50">
-        <v>0</v>
-      </c>
-      <c r="M50">
-        <v>0</v>
-      </c>
-      <c r="N50">
-        <v>0</v>
-      </c>
-      <c r="O50">
-        <v>0</v>
-      </c>
-      <c r="P50">
-        <v>0</v>
-      </c>
-      <c r="Q50">
+      <c r="L50" s="18">
+        <v>0</v>
+      </c>
+      <c r="M50" s="18">
+        <v>0</v>
+      </c>
+      <c r="N50" s="18">
+        <v>0</v>
+      </c>
+      <c r="O50" s="18">
+        <v>0</v>
+      </c>
+      <c r="P50" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q50" s="18">
         <f t="shared" si="0"/>
         <v>1160000</v>
       </c>
@@ -3761,37 +3769,37 @@
       <c r="F51" t="s">
         <v>215</v>
       </c>
-      <c r="G51">
+      <c r="G51" s="18">
         <v>5200000</v>
       </c>
-      <c r="H51">
+      <c r="H51" s="18">
         <v>1900000</v>
       </c>
-      <c r="I51">
+      <c r="I51" s="18">
         <v>520000</v>
       </c>
-      <c r="J51">
+      <c r="J51" s="18">
         <v>620000</v>
       </c>
-      <c r="K51">
+      <c r="K51" s="18">
         <v>1200000</v>
       </c>
-      <c r="L51">
+      <c r="L51" s="18">
         <v>960000</v>
       </c>
-      <c r="M51">
-        <v>0</v>
-      </c>
-      <c r="N51">
-        <v>0</v>
-      </c>
-      <c r="O51">
-        <v>0</v>
-      </c>
-      <c r="P51">
+      <c r="M51" s="18">
+        <v>0</v>
+      </c>
+      <c r="N51" s="18">
+        <v>0</v>
+      </c>
+      <c r="O51" s="18">
+        <v>0</v>
+      </c>
+      <c r="P51" s="18">
         <v>2400000</v>
       </c>
-      <c r="Q51">
+      <c r="Q51" s="18">
         <f t="shared" si="0"/>
         <v>12800000</v>
       </c>
@@ -3813,37 +3821,37 @@
       <c r="F52" t="s">
         <v>217</v>
       </c>
-      <c r="G52">
+      <c r="G52" s="18">
         <v>1400000</v>
       </c>
-      <c r="H52">
-        <v>0</v>
-      </c>
-      <c r="I52">
+      <c r="H52" s="18">
+        <v>0</v>
+      </c>
+      <c r="I52" s="18">
         <v>140000</v>
       </c>
-      <c r="J52">
+      <c r="J52" s="18">
         <v>200000</v>
       </c>
-      <c r="K52">
-        <v>0</v>
-      </c>
-      <c r="L52">
+      <c r="K52" s="18">
+        <v>0</v>
+      </c>
+      <c r="L52" s="18">
         <v>260000</v>
       </c>
-      <c r="M52">
-        <v>0</v>
-      </c>
-      <c r="N52">
-        <v>0</v>
-      </c>
-      <c r="O52">
-        <v>0</v>
-      </c>
-      <c r="P52">
+      <c r="M52" s="18">
+        <v>0</v>
+      </c>
+      <c r="N52" s="18">
+        <v>0</v>
+      </c>
+      <c r="O52" s="18">
+        <v>0</v>
+      </c>
+      <c r="P52" s="18">
         <v>950000</v>
       </c>
-      <c r="Q52">
+      <c r="Q52" s="18">
         <f t="shared" si="0"/>
         <v>2950000</v>
       </c>
@@ -3865,37 +3873,37 @@
       <c r="F53" t="s">
         <v>219</v>
       </c>
-      <c r="G53">
+      <c r="G53" s="18">
         <v>1080000</v>
       </c>
-      <c r="H53">
-        <v>0</v>
-      </c>
-      <c r="I53">
+      <c r="H53" s="18">
+        <v>0</v>
+      </c>
+      <c r="I53" s="18">
         <v>108000</v>
       </c>
-      <c r="J53">
+      <c r="J53" s="18">
         <v>165000</v>
       </c>
-      <c r="K53">
-        <v>0</v>
-      </c>
-      <c r="L53">
+      <c r="K53" s="18">
+        <v>0</v>
+      </c>
+      <c r="L53" s="18">
         <v>197000</v>
       </c>
-      <c r="M53">
-        <v>0</v>
-      </c>
-      <c r="N53">
-        <v>0</v>
-      </c>
-      <c r="O53">
-        <v>0</v>
-      </c>
-      <c r="P53">
+      <c r="M53" s="18">
+        <v>0</v>
+      </c>
+      <c r="N53" s="18">
+        <v>0</v>
+      </c>
+      <c r="O53" s="18">
+        <v>0</v>
+      </c>
+      <c r="P53" s="18">
         <v>750000</v>
       </c>
-      <c r="Q53">
+      <c r="Q53" s="18">
         <f t="shared" si="0"/>
         <v>2300000</v>
       </c>
@@ -3917,37 +3925,37 @@
       <c r="F54" t="s">
         <v>221</v>
       </c>
-      <c r="G54">
+      <c r="G54" s="18">
         <v>920000</v>
       </c>
-      <c r="H54">
-        <v>0</v>
-      </c>
-      <c r="I54">
+      <c r="H54" s="18">
+        <v>0</v>
+      </c>
+      <c r="I54" s="18">
         <v>92000</v>
       </c>
-      <c r="J54">
+      <c r="J54" s="18">
         <v>140000</v>
       </c>
-      <c r="K54">
-        <v>0</v>
-      </c>
-      <c r="L54">
+      <c r="K54" s="18">
+        <v>0</v>
+      </c>
+      <c r="L54" s="18">
         <v>168000</v>
       </c>
-      <c r="M54">
-        <v>0</v>
-      </c>
-      <c r="N54">
-        <v>0</v>
-      </c>
-      <c r="O54">
-        <v>0</v>
-      </c>
-      <c r="P54">
+      <c r="M54" s="18">
+        <v>0</v>
+      </c>
+      <c r="N54" s="18">
+        <v>0</v>
+      </c>
+      <c r="O54" s="18">
+        <v>0</v>
+      </c>
+      <c r="P54" s="18">
         <v>650000</v>
       </c>
-      <c r="Q54">
+      <c r="Q54" s="18">
         <f t="shared" si="0"/>
         <v>1970000</v>
       </c>
@@ -3969,37 +3977,37 @@
       <c r="F55" t="s">
         <v>223</v>
       </c>
-      <c r="G55">
+      <c r="G55" s="18">
         <v>3300000</v>
       </c>
-      <c r="H55">
+      <c r="H55" s="18">
         <v>1200000</v>
       </c>
-      <c r="I55">
+      <c r="I55" s="18">
         <v>330000</v>
       </c>
-      <c r="J55">
+      <c r="J55" s="18">
         <v>390000</v>
       </c>
-      <c r="K55">
+      <c r="K55" s="18">
         <v>780000</v>
       </c>
-      <c r="L55">
+      <c r="L55" s="18">
         <v>600000</v>
       </c>
-      <c r="M55">
-        <v>0</v>
-      </c>
-      <c r="N55">
-        <v>0</v>
-      </c>
-      <c r="O55">
-        <v>0</v>
-      </c>
-      <c r="P55">
+      <c r="M55" s="18">
+        <v>0</v>
+      </c>
+      <c r="N55" s="18">
+        <v>0</v>
+      </c>
+      <c r="O55" s="18">
+        <v>0</v>
+      </c>
+      <c r="P55" s="18">
         <v>1900000</v>
       </c>
-      <c r="Q55">
+      <c r="Q55" s="18">
         <f t="shared" si="0"/>
         <v>8500000</v>
       </c>
@@ -4021,37 +4029,37 @@
       <c r="F56" t="s">
         <v>225</v>
       </c>
-      <c r="G56">
+      <c r="G56" s="18">
         <v>780000</v>
       </c>
-      <c r="H56">
+      <c r="H56" s="18">
         <v>230000</v>
       </c>
-      <c r="I56">
+      <c r="I56" s="18">
         <v>40000</v>
       </c>
-      <c r="J56">
+      <c r="J56" s="18">
         <v>360000</v>
       </c>
-      <c r="K56">
+      <c r="K56" s="18">
         <v>150000</v>
       </c>
-      <c r="L56">
-        <v>0</v>
-      </c>
-      <c r="M56">
-        <v>0</v>
-      </c>
-      <c r="N56">
-        <v>0</v>
-      </c>
-      <c r="O56">
-        <v>0</v>
-      </c>
-      <c r="P56">
-        <v>0</v>
-      </c>
-      <c r="Q56">
+      <c r="L56" s="18">
+        <v>0</v>
+      </c>
+      <c r="M56" s="18">
+        <v>0</v>
+      </c>
+      <c r="N56" s="18">
+        <v>0</v>
+      </c>
+      <c r="O56" s="18">
+        <v>0</v>
+      </c>
+      <c r="P56" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q56" s="18">
         <f t="shared" si="0"/>
         <v>1560000</v>
       </c>
@@ -4073,37 +4081,37 @@
       <c r="F57" t="s">
         <v>227</v>
       </c>
-      <c r="G57">
+      <c r="G57" s="18">
         <v>980000</v>
       </c>
-      <c r="H57">
+      <c r="H57" s="18">
         <v>290000</v>
       </c>
-      <c r="I57">
+      <c r="I57" s="18">
         <v>48000</v>
       </c>
-      <c r="J57">
+      <c r="J57" s="18">
         <v>450000</v>
       </c>
-      <c r="K57">
+      <c r="K57" s="18">
         <v>192000</v>
       </c>
-      <c r="L57">
-        <v>0</v>
-      </c>
-      <c r="M57">
-        <v>0</v>
-      </c>
-      <c r="N57">
-        <v>0</v>
-      </c>
-      <c r="O57">
-        <v>0</v>
-      </c>
-      <c r="P57">
-        <v>0</v>
-      </c>
-      <c r="Q57">
+      <c r="L57" s="18">
+        <v>0</v>
+      </c>
+      <c r="M57" s="18">
+        <v>0</v>
+      </c>
+      <c r="N57" s="18">
+        <v>0</v>
+      </c>
+      <c r="O57" s="18">
+        <v>0</v>
+      </c>
+      <c r="P57" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q57" s="18">
         <f t="shared" si="0"/>
         <v>1960000</v>
       </c>
@@ -4125,37 +4133,37 @@
       <c r="F58" t="s">
         <v>229</v>
       </c>
-      <c r="G58">
+      <c r="G58" s="18">
         <v>620000</v>
       </c>
-      <c r="H58">
+      <c r="H58" s="18">
         <v>180000</v>
       </c>
-      <c r="I58">
+      <c r="I58" s="18">
         <v>32000</v>
       </c>
-      <c r="J58">
+      <c r="J58" s="18">
         <v>285000</v>
       </c>
-      <c r="K58">
+      <c r="K58" s="18">
         <v>123000</v>
       </c>
-      <c r="L58">
-        <v>0</v>
-      </c>
-      <c r="M58">
-        <v>0</v>
-      </c>
-      <c r="N58">
-        <v>0</v>
-      </c>
-      <c r="O58">
-        <v>0</v>
-      </c>
-      <c r="P58">
-        <v>0</v>
-      </c>
-      <c r="Q58">
+      <c r="L58" s="18">
+        <v>0</v>
+      </c>
+      <c r="M58" s="18">
+        <v>0</v>
+      </c>
+      <c r="N58" s="18">
+        <v>0</v>
+      </c>
+      <c r="O58" s="18">
+        <v>0</v>
+      </c>
+      <c r="P58" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q58" s="18">
         <f t="shared" si="0"/>
         <v>1240000</v>
       </c>
@@ -4177,37 +4185,37 @@
       <c r="F59" t="s">
         <v>231</v>
       </c>
-      <c r="G59">
+      <c r="G59" s="18">
         <v>850000</v>
       </c>
-      <c r="H59">
+      <c r="H59" s="18">
         <v>250000</v>
       </c>
-      <c r="I59">
+      <c r="I59" s="18">
         <v>42000</v>
       </c>
-      <c r="J59">
+      <c r="J59" s="18">
         <v>390000</v>
       </c>
-      <c r="K59">
+      <c r="K59" s="18">
         <v>168000</v>
       </c>
-      <c r="L59">
-        <v>0</v>
-      </c>
-      <c r="M59">
-        <v>0</v>
-      </c>
-      <c r="N59">
-        <v>0</v>
-      </c>
-      <c r="O59">
-        <v>0</v>
-      </c>
-      <c r="P59">
-        <v>0</v>
-      </c>
-      <c r="Q59">
+      <c r="L59" s="18">
+        <v>0</v>
+      </c>
+      <c r="M59" s="18">
+        <v>0</v>
+      </c>
+      <c r="N59" s="18">
+        <v>0</v>
+      </c>
+      <c r="O59" s="18">
+        <v>0</v>
+      </c>
+      <c r="P59" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q59" s="18">
         <f t="shared" si="0"/>
         <v>1700000</v>
       </c>
@@ -4229,37 +4237,37 @@
       <c r="F60" t="s">
         <v>233</v>
       </c>
-      <c r="G60">
+      <c r="G60" s="18">
         <v>690000</v>
       </c>
-      <c r="H60">
+      <c r="H60" s="18">
         <v>200000</v>
       </c>
-      <c r="I60">
+      <c r="I60" s="18">
         <v>35000</v>
       </c>
-      <c r="J60">
+      <c r="J60" s="18">
         <v>315000</v>
       </c>
-      <c r="K60">
+      <c r="K60" s="18">
         <v>140000</v>
       </c>
-      <c r="L60">
-        <v>0</v>
-      </c>
-      <c r="M60">
-        <v>0</v>
-      </c>
-      <c r="N60">
-        <v>0</v>
-      </c>
-      <c r="O60">
-        <v>0</v>
-      </c>
-      <c r="P60">
-        <v>0</v>
-      </c>
-      <c r="Q60">
+      <c r="L60" s="18">
+        <v>0</v>
+      </c>
+      <c r="M60" s="18">
+        <v>0</v>
+      </c>
+      <c r="N60" s="18">
+        <v>0</v>
+      </c>
+      <c r="O60" s="18">
+        <v>0</v>
+      </c>
+      <c r="P60" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q60" s="18">
         <f t="shared" si="0"/>
         <v>1380000</v>
       </c>
@@ -4281,37 +4289,37 @@
       <c r="F61" t="s">
         <v>235</v>
       </c>
-      <c r="G61">
+      <c r="G61" s="18">
         <v>480000</v>
       </c>
-      <c r="H61">
+      <c r="H61" s="18">
         <v>140000</v>
       </c>
-      <c r="I61">
+      <c r="I61" s="18">
         <v>25000</v>
       </c>
-      <c r="J61">
+      <c r="J61" s="18">
         <v>220000</v>
       </c>
-      <c r="K61">
+      <c r="K61" s="18">
         <v>95000</v>
       </c>
-      <c r="L61">
-        <v>0</v>
-      </c>
-      <c r="M61">
-        <v>0</v>
-      </c>
-      <c r="N61">
-        <v>0</v>
-      </c>
-      <c r="O61">
-        <v>0</v>
-      </c>
-      <c r="P61">
-        <v>0</v>
-      </c>
-      <c r="Q61">
+      <c r="L61" s="18">
+        <v>0</v>
+      </c>
+      <c r="M61" s="18">
+        <v>0</v>
+      </c>
+      <c r="N61" s="18">
+        <v>0</v>
+      </c>
+      <c r="O61" s="18">
+        <v>0</v>
+      </c>
+      <c r="P61" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q61" s="18">
         <f t="shared" si="0"/>
         <v>960000</v>
       </c>
@@ -4333,37 +4341,37 @@
       <c r="F62" t="s">
         <v>237</v>
       </c>
-      <c r="G62">
+      <c r="G62" s="18">
         <v>520000</v>
       </c>
-      <c r="H62">
+      <c r="H62" s="18">
         <v>152000</v>
       </c>
-      <c r="I62">
+      <c r="I62" s="18">
         <v>27000</v>
       </c>
-      <c r="J62">
+      <c r="J62" s="18">
         <v>238000</v>
       </c>
-      <c r="K62">
+      <c r="K62" s="18">
         <v>103000</v>
       </c>
-      <c r="L62">
-        <v>0</v>
-      </c>
-      <c r="M62">
-        <v>0</v>
-      </c>
-      <c r="N62">
-        <v>0</v>
-      </c>
-      <c r="O62">
-        <v>0</v>
-      </c>
-      <c r="P62">
-        <v>0</v>
-      </c>
-      <c r="Q62">
+      <c r="L62" s="18">
+        <v>0</v>
+      </c>
+      <c r="M62" s="18">
+        <v>0</v>
+      </c>
+      <c r="N62" s="18">
+        <v>0</v>
+      </c>
+      <c r="O62" s="18">
+        <v>0</v>
+      </c>
+      <c r="P62" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q62" s="18">
         <f t="shared" si="0"/>
         <v>1040000</v>
       </c>
@@ -4385,37 +4393,37 @@
       <c r="F63" t="s">
         <v>239</v>
       </c>
-      <c r="G63">
+      <c r="G63" s="18">
         <v>420000</v>
       </c>
-      <c r="H63">
+      <c r="H63" s="18">
         <v>122000</v>
       </c>
-      <c r="I63">
+      <c r="I63" s="18">
         <v>22000</v>
       </c>
-      <c r="J63">
+      <c r="J63" s="18">
         <v>192000</v>
       </c>
-      <c r="K63">
+      <c r="K63" s="18">
         <v>84000</v>
       </c>
-      <c r="L63">
-        <v>0</v>
-      </c>
-      <c r="M63">
-        <v>0</v>
-      </c>
-      <c r="N63">
-        <v>0</v>
-      </c>
-      <c r="O63">
-        <v>0</v>
-      </c>
-      <c r="P63">
-        <v>0</v>
-      </c>
-      <c r="Q63">
+      <c r="L63" s="18">
+        <v>0</v>
+      </c>
+      <c r="M63" s="18">
+        <v>0</v>
+      </c>
+      <c r="N63" s="18">
+        <v>0</v>
+      </c>
+      <c r="O63" s="18">
+        <v>0</v>
+      </c>
+      <c r="P63" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q63" s="18">
         <f t="shared" si="0"/>
         <v>840000</v>
       </c>
@@ -4437,37 +4445,37 @@
       <c r="F64" t="s">
         <v>241</v>
       </c>
-      <c r="G64">
+      <c r="G64" s="18">
         <v>580000</v>
       </c>
-      <c r="H64">
+      <c r="H64" s="18">
         <v>170000</v>
       </c>
-      <c r="I64">
+      <c r="I64" s="18">
         <v>30000</v>
       </c>
-      <c r="J64">
+      <c r="J64" s="18">
         <v>265000</v>
       </c>
-      <c r="K64">
+      <c r="K64" s="18">
         <v>115000</v>
       </c>
-      <c r="L64">
-        <v>0</v>
-      </c>
-      <c r="M64">
-        <v>0</v>
-      </c>
-      <c r="N64">
-        <v>0</v>
-      </c>
-      <c r="O64">
-        <v>0</v>
-      </c>
-      <c r="P64">
-        <v>0</v>
-      </c>
-      <c r="Q64">
+      <c r="L64" s="18">
+        <v>0</v>
+      </c>
+      <c r="M64" s="18">
+        <v>0</v>
+      </c>
+      <c r="N64" s="18">
+        <v>0</v>
+      </c>
+      <c r="O64" s="18">
+        <v>0</v>
+      </c>
+      <c r="P64" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q64" s="18">
         <f t="shared" si="0"/>
         <v>1160000</v>
       </c>
@@ -4489,37 +4497,37 @@
       <c r="F65" t="s">
         <v>243</v>
       </c>
-      <c r="G65">
+      <c r="G65" s="18">
         <v>680000</v>
       </c>
-      <c r="H65">
-        <v>0</v>
-      </c>
-      <c r="I65">
+      <c r="H65" s="18">
+        <v>0</v>
+      </c>
+      <c r="I65" s="18">
         <v>68000</v>
       </c>
-      <c r="J65">
+      <c r="J65" s="18">
         <v>105000</v>
       </c>
-      <c r="K65">
-        <v>0</v>
-      </c>
-      <c r="L65">
+      <c r="K65" s="18">
+        <v>0</v>
+      </c>
+      <c r="L65" s="18">
         <v>127000</v>
       </c>
-      <c r="M65">
-        <v>0</v>
-      </c>
-      <c r="N65">
-        <v>0</v>
-      </c>
-      <c r="O65">
-        <v>0</v>
-      </c>
-      <c r="P65">
+      <c r="M65" s="18">
+        <v>0</v>
+      </c>
+      <c r="N65" s="18">
+        <v>0</v>
+      </c>
+      <c r="O65" s="18">
+        <v>0</v>
+      </c>
+      <c r="P65" s="18">
         <v>520000</v>
       </c>
-      <c r="Q65">
+      <c r="Q65" s="18">
         <f t="shared" si="0"/>
         <v>1500000</v>
       </c>
@@ -4541,37 +4549,37 @@
       <c r="F66" t="s">
         <v>245</v>
       </c>
-      <c r="G66">
+      <c r="G66" s="18">
         <v>2800000</v>
       </c>
-      <c r="H66">
-        <v>0</v>
-      </c>
-      <c r="I66">
+      <c r="H66" s="18">
+        <v>0</v>
+      </c>
+      <c r="I66" s="18">
         <v>280000</v>
       </c>
-      <c r="J66">
+      <c r="J66" s="18">
         <v>410000</v>
       </c>
-      <c r="K66">
-        <v>0</v>
-      </c>
-      <c r="L66">
+      <c r="K66" s="18">
+        <v>0</v>
+      </c>
+      <c r="L66" s="18">
         <v>530000</v>
       </c>
-      <c r="M66">
-        <v>0</v>
-      </c>
-      <c r="N66">
-        <v>0</v>
-      </c>
-      <c r="O66">
-        <v>0</v>
-      </c>
-      <c r="P66">
+      <c r="M66" s="18">
+        <v>0</v>
+      </c>
+      <c r="N66" s="18">
+        <v>0</v>
+      </c>
+      <c r="O66" s="18">
+        <v>0</v>
+      </c>
+      <c r="P66" s="18">
         <v>1900000</v>
       </c>
-      <c r="Q66">
+      <c r="Q66" s="18">
         <f t="shared" si="0"/>
         <v>5920000</v>
       </c>
@@ -4593,37 +4601,37 @@
       <c r="F67" t="s">
         <v>247</v>
       </c>
-      <c r="G67">
+      <c r="G67" s="18">
         <v>2200000</v>
       </c>
-      <c r="H67">
-        <v>0</v>
-      </c>
-      <c r="I67">
+      <c r="H67" s="18">
+        <v>0</v>
+      </c>
+      <c r="I67" s="18">
         <v>220000</v>
       </c>
-      <c r="J67">
+      <c r="J67" s="18">
         <v>320000</v>
       </c>
-      <c r="K67">
-        <v>0</v>
-      </c>
-      <c r="L67">
+      <c r="K67" s="18">
+        <v>0</v>
+      </c>
+      <c r="L67" s="18">
         <v>440000</v>
       </c>
-      <c r="M67">
-        <v>0</v>
-      </c>
-      <c r="N67">
-        <v>0</v>
-      </c>
-      <c r="O67">
-        <v>0</v>
-      </c>
-      <c r="P67">
+      <c r="M67" s="18">
+        <v>0</v>
+      </c>
+      <c r="N67" s="18">
+        <v>0</v>
+      </c>
+      <c r="O67" s="18">
+        <v>0</v>
+      </c>
+      <c r="P67" s="18">
         <v>1500000</v>
       </c>
-      <c r="Q67">
+      <c r="Q67" s="18">
         <f t="shared" si="0"/>
         <v>4680000</v>
       </c>
@@ -4645,37 +4653,37 @@
       <c r="F68" t="s">
         <v>249</v>
       </c>
-      <c r="G68">
+      <c r="G68" s="18">
         <v>2500000</v>
       </c>
-      <c r="H68">
-        <v>0</v>
-      </c>
-      <c r="I68">
+      <c r="H68" s="18">
+        <v>0</v>
+      </c>
+      <c r="I68" s="18">
         <v>250000</v>
       </c>
-      <c r="J68">
+      <c r="J68" s="18">
         <v>370000</v>
       </c>
-      <c r="K68">
-        <v>0</v>
-      </c>
-      <c r="L68">
+      <c r="K68" s="18">
+        <v>0</v>
+      </c>
+      <c r="L68" s="18">
         <v>480000</v>
       </c>
-      <c r="M68">
-        <v>0</v>
-      </c>
-      <c r="N68">
-        <v>0</v>
-      </c>
-      <c r="O68">
-        <v>0</v>
-      </c>
-      <c r="P68">
+      <c r="M68" s="18">
+        <v>0</v>
+      </c>
+      <c r="N68" s="18">
+        <v>0</v>
+      </c>
+      <c r="O68" s="18">
+        <v>0</v>
+      </c>
+      <c r="P68" s="18">
         <v>1700000</v>
       </c>
-      <c r="Q68">
+      <c r="Q68" s="18">
         <f t="shared" si="0"/>
         <v>5300000</v>
       </c>
@@ -4697,37 +4705,37 @@
       <c r="F69" t="s">
         <v>251</v>
       </c>
-      <c r="G69">
+      <c r="G69" s="18">
         <v>1100000</v>
       </c>
-      <c r="H69">
-        <v>0</v>
-      </c>
-      <c r="I69">
+      <c r="H69" s="18">
+        <v>0</v>
+      </c>
+      <c r="I69" s="18">
         <v>110000</v>
       </c>
-      <c r="J69">
+      <c r="J69" s="18">
         <v>165000</v>
       </c>
-      <c r="K69">
-        <v>0</v>
-      </c>
-      <c r="L69">
+      <c r="K69" s="18">
+        <v>0</v>
+      </c>
+      <c r="L69" s="18">
         <v>225000</v>
       </c>
-      <c r="M69">
-        <v>0</v>
-      </c>
-      <c r="N69">
-        <v>0</v>
-      </c>
-      <c r="O69">
-        <v>0</v>
-      </c>
-      <c r="P69">
+      <c r="M69" s="18">
+        <v>0</v>
+      </c>
+      <c r="N69" s="18">
+        <v>0</v>
+      </c>
+      <c r="O69" s="18">
+        <v>0</v>
+      </c>
+      <c r="P69" s="18">
         <v>780000</v>
       </c>
-      <c r="Q69">
+      <c r="Q69" s="18">
         <f t="shared" si="0"/>
         <v>2380000</v>
       </c>
@@ -4749,124 +4757,124 @@
       <c r="F70" t="s">
         <v>253</v>
       </c>
-      <c r="G70">
+      <c r="G70" s="18">
         <v>780000</v>
       </c>
-      <c r="H70">
-        <v>0</v>
-      </c>
-      <c r="I70">
+      <c r="H70" s="18">
+        <v>0</v>
+      </c>
+      <c r="I70" s="18">
         <v>78000</v>
       </c>
-      <c r="J70">
+      <c r="J70" s="18">
         <v>118000</v>
       </c>
-      <c r="K70">
-        <v>0</v>
-      </c>
-      <c r="L70">
+      <c r="K70" s="18">
+        <v>0</v>
+      </c>
+      <c r="L70" s="18">
         <v>154000</v>
       </c>
-      <c r="M70">
-        <v>0</v>
-      </c>
-      <c r="N70">
-        <v>0</v>
-      </c>
-      <c r="O70">
-        <v>0</v>
-      </c>
-      <c r="P70">
+      <c r="M70" s="18">
+        <v>0</v>
+      </c>
+      <c r="N70" s="18">
+        <v>0</v>
+      </c>
+      <c r="O70" s="18">
+        <v>0</v>
+      </c>
+      <c r="P70" s="18">
         <v>550000</v>
       </c>
-      <c r="Q70">
+      <c r="Q70" s="18">
         <f t="shared" si="0"/>
         <v>1680000</v>
       </c>
     </row>
     <row r="71" spans="1:47" ht="14.5" customHeight="1" outlineLevel="1">
-      <c r="B71" s="12"/>
-      <c r="C71" s="12"/>
-      <c r="D71" s="12"/>
-      <c r="E71" s="12"/>
-      <c r="F71" s="12"/>
-      <c r="G71" s="12"/>
-      <c r="H71" s="12"/>
-      <c r="I71" s="12"/>
-      <c r="J71" s="12"/>
-      <c r="K71" s="12"/>
-      <c r="L71" s="12"/>
-      <c r="M71" s="12"/>
-      <c r="N71" s="12"/>
-      <c r="O71" s="12"/>
-      <c r="P71" s="12"/>
-      <c r="Q71" s="12"/>
+      <c r="B71" s="11"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="11"/>
+      <c r="E71" s="11"/>
+      <c r="F71" s="11"/>
+      <c r="G71" s="11"/>
+      <c r="H71" s="11"/>
+      <c r="I71" s="11"/>
+      <c r="J71" s="11"/>
+      <c r="K71" s="11"/>
+      <c r="L71" s="11"/>
+      <c r="M71" s="11"/>
+      <c r="N71" s="11"/>
+      <c r="O71" s="11"/>
+      <c r="P71" s="11"/>
+      <c r="Q71" s="11"/>
     </row>
     <row r="72" spans="1:47" ht="14.5" customHeight="1">
-      <c r="B72" s="17" t="s">
+      <c r="B72" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C72" s="17"/>
-      <c r="D72" s="17"/>
-      <c r="E72" s="13"/>
-      <c r="F72" s="13"/>
-      <c r="G72" s="10">
+      <c r="C72" s="15"/>
+      <c r="D72" s="15"/>
+      <c r="E72" s="12"/>
+      <c r="F72" s="12"/>
+      <c r="G72" s="19">
         <f t="shared" ref="G72:P72" si="1">SUM(G7:G70)</f>
         <v>360620000</v>
       </c>
-      <c r="H72" s="10">
+      <c r="H72" s="19">
         <f t="shared" si="1"/>
         <v>118954000</v>
       </c>
-      <c r="I72" s="10">
+      <c r="I72" s="19">
         <f t="shared" si="1"/>
         <v>34784000</v>
       </c>
-      <c r="J72" s="10">
+      <c r="J72" s="19">
         <f t="shared" si="1"/>
         <v>39663000</v>
       </c>
-      <c r="K72" s="10">
+      <c r="K72" s="19">
         <f t="shared" si="1"/>
         <v>47997000</v>
       </c>
-      <c r="L72" s="10">
+      <c r="L72" s="19">
         <f t="shared" si="1"/>
         <v>60632000</v>
       </c>
-      <c r="M72" s="10">
+      <c r="M72" s="19">
         <f t="shared" si="1"/>
         <v>37100000</v>
       </c>
-      <c r="N72" s="10">
+      <c r="N72" s="19">
         <f t="shared" si="1"/>
         <v>3500000</v>
       </c>
-      <c r="O72" s="10">
+      <c r="O72" s="19">
         <f t="shared" si="1"/>
         <v>2950000</v>
       </c>
-      <c r="P72" s="10">
+      <c r="P72" s="19">
         <f t="shared" si="1"/>
         <v>96380000</v>
       </c>
-      <c r="Q72" s="10">
+      <c r="Q72" s="19">
         <f>SUM(Q7:Q70)</f>
         <v>802580000</v>
       </c>
     </row>
     <row r="73" spans="1:47">
-      <c r="G73" s="15"/>
-      <c r="H73" s="15"/>
-      <c r="I73" s="15"/>
-      <c r="J73" s="15"/>
-      <c r="K73" s="15"/>
-      <c r="L73" s="15"/>
-      <c r="M73" s="15"/>
-      <c r="N73" s="15"/>
-      <c r="O73" s="15"/>
-      <c r="P73" s="15"/>
-      <c r="Q73" s="15"/>
+      <c r="G73" s="14"/>
+      <c r="H73" s="14"/>
+      <c r="I73" s="14"/>
+      <c r="J73" s="14"/>
+      <c r="K73" s="14"/>
+      <c r="L73" s="14"/>
+      <c r="M73" s="14"/>
+      <c r="N73" s="14"/>
+      <c r="O73" s="14"/>
+      <c r="P73" s="14"/>
+      <c r="Q73" s="14"/>
     </row>
     <row r="74" spans="1:47">
       <c r="F74"/>
@@ -4898,7 +4906,7 @@
     <row r="76" spans="1:47">
       <c r="A76" s="1"/>
       <c r="C76" s="4"/>
-      <c r="N76" s="14"/>
+      <c r="N76" s="13"/>
     </row>
     <row r="77" spans="1:47" s="1" customFormat="1">
       <c r="C77" s="4"/>
@@ -5352,15 +5360,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="72e9687c-dd16-42a4-b22f-37506a5a0d78" xsi:nil="true"/>
@@ -5369,6 +5368,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5391,14 +5399,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2544B30-2F4A-4C87-AE99-36BD3CF47B15}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D5EA2B3-D5F1-4BCA-8B03-ACB94ED8953E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -5409,4 +5409,12 @@
     <ds:schemaRef ds:uri="ca11ca2f-01e5-493b-bb15-47564d08beeb"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2544B30-2F4A-4C87-AE99-36BD3CF47B15}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>